<commit_message>
completando a taela Target
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Documents\GitHub\22-2b-cd-p1-grupo_joaoogp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b866b217d0e5359/Área de Trabalho/Insper/2o semestre/Ciência dos Dados/Projeto 1/22-2b-cd-p1-grupo_joaoogp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFCFE07-6B38-4DB7-9263-61A542C365A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{6AFCFE07-6B38-4DB7-9263-61A542C365A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC0251BC-59D5-40B6-850B-1F0323FF5BD1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18115,8 +18115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A791" workbookViewId="0">
-      <selection activeCell="K803" sqref="K803"/>
+    <sheetView tabSelected="1" topLeftCell="A1076" workbookViewId="0">
+      <selection activeCell="O1094" sqref="O1094"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39048,7 +39048,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="1089" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1089" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1089" t="s">
         <v>6</v>
       </c>
@@ -39065,7 +39065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1090" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1090" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1090" t="s">
         <v>6</v>
       </c>
@@ -39082,7 +39082,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="1091" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1091" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1091" t="s">
         <v>6</v>
       </c>
@@ -39099,7 +39099,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1092" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1092" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1092" t="s">
         <v>6</v>
       </c>
@@ -39116,7 +39116,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1093" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1093" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1093" t="s">
         <v>6</v>
       </c>
@@ -39133,7 +39133,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1094" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1094" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1094" t="s">
         <v>6</v>
       </c>
@@ -39149,8 +39149,11 @@
       <c r="E1094">
         <v>57</v>
       </c>
-    </row>
-    <row r="1095" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1094">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1095" t="s">
         <v>6</v>
       </c>
@@ -39166,8 +39169,11 @@
       <c r="E1095">
         <v>23</v>
       </c>
-    </row>
-    <row r="1096" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1095">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1096" t="s">
         <v>6</v>
       </c>
@@ -39183,8 +39189,11 @@
       <c r="E1096">
         <v>39</v>
       </c>
-    </row>
-    <row r="1097" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1096">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1097" t="s">
         <v>6</v>
       </c>
@@ -39200,8 +39209,11 @@
       <c r="E1097">
         <v>47</v>
       </c>
-    </row>
-    <row r="1098" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1097">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1098" t="s">
         <v>6</v>
       </c>
@@ -39217,8 +39229,11 @@
       <c r="E1098">
         <v>90</v>
       </c>
-    </row>
-    <row r="1099" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1098">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1099" t="s">
         <v>6</v>
       </c>
@@ -39234,8 +39249,11 @@
       <c r="E1099">
         <v>2</v>
       </c>
-    </row>
-    <row r="1100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1099">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1100" t="s">
         <v>6</v>
       </c>
@@ -39251,8 +39269,11 @@
       <c r="E1100">
         <v>23</v>
       </c>
-    </row>
-    <row r="1101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1101" t="s">
         <v>6</v>
       </c>
@@ -39268,8 +39289,11 @@
       <c r="E1101">
         <v>62</v>
       </c>
-    </row>
-    <row r="1102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1102" t="s">
         <v>6</v>
       </c>
@@ -39285,8 +39309,11 @@
       <c r="E1102">
         <v>96</v>
       </c>
-    </row>
-    <row r="1103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1103" t="s">
         <v>6</v>
       </c>
@@ -39302,8 +39329,11 @@
       <c r="E1103">
         <v>42</v>
       </c>
-    </row>
-    <row r="1104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1104" t="s">
         <v>6</v>
       </c>
@@ -39319,8 +39349,11 @@
       <c r="E1104">
         <v>66</v>
       </c>
-    </row>
-    <row r="1105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1105" t="s">
         <v>6</v>
       </c>
@@ -39336,8 +39369,11 @@
       <c r="E1105">
         <v>5</v>
       </c>
-    </row>
-    <row r="1106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1106" t="s">
         <v>6</v>
       </c>
@@ -39353,8 +39389,11 @@
       <c r="E1106">
         <v>1</v>
       </c>
-    </row>
-    <row r="1107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1107" t="s">
         <v>6</v>
       </c>
@@ -39370,8 +39409,11 @@
       <c r="E1107">
         <v>65</v>
       </c>
-    </row>
-    <row r="1108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1108" t="s">
         <v>6</v>
       </c>
@@ -39387,8 +39429,11 @@
       <c r="E1108">
         <v>64</v>
       </c>
-    </row>
-    <row r="1109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1109" t="s">
         <v>6</v>
       </c>
@@ -39404,8 +39449,11 @@
       <c r="E1109">
         <v>61</v>
       </c>
-    </row>
-    <row r="1110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1110" t="s">
         <v>6</v>
       </c>
@@ -39421,8 +39469,11 @@
       <c r="E1110">
         <v>20</v>
       </c>
-    </row>
-    <row r="1111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1111" t="s">
         <v>6</v>
       </c>
@@ -39438,8 +39489,11 @@
       <c r="E1111">
         <v>40</v>
       </c>
-    </row>
-    <row r="1112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1112" t="s">
         <v>6</v>
       </c>
@@ -39455,8 +39509,11 @@
       <c r="E1112">
         <v>95</v>
       </c>
-    </row>
-    <row r="1113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1113" t="s">
         <v>6</v>
       </c>
@@ -39472,8 +39529,11 @@
       <c r="E1113">
         <v>5</v>
       </c>
-    </row>
-    <row r="1114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1114" t="s">
         <v>6</v>
       </c>
@@ -39489,8 +39549,11 @@
       <c r="E1114">
         <v>84</v>
       </c>
-    </row>
-    <row r="1115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1115" t="s">
         <v>6</v>
       </c>
@@ -39506,8 +39569,11 @@
       <c r="E1115">
         <v>9</v>
       </c>
-    </row>
-    <row r="1116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1116" t="s">
         <v>6</v>
       </c>
@@ -39523,8 +39589,11 @@
       <c r="E1116">
         <v>99</v>
       </c>
-    </row>
-    <row r="1117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1117" t="s">
         <v>6</v>
       </c>
@@ -39540,8 +39609,11 @@
       <c r="E1117">
         <v>68</v>
       </c>
-    </row>
-    <row r="1118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1118" t="s">
         <v>6</v>
       </c>
@@ -39557,8 +39629,11 @@
       <c r="E1118">
         <v>87</v>
       </c>
-    </row>
-    <row r="1119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1119" t="s">
         <v>6</v>
       </c>
@@ -39574,8 +39649,11 @@
       <c r="E1119">
         <v>10</v>
       </c>
-    </row>
-    <row r="1120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1120" t="s">
         <v>6</v>
       </c>
@@ -39591,8 +39669,11 @@
       <c r="E1120">
         <v>51</v>
       </c>
-    </row>
-    <row r="1121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1121" t="s">
         <v>6</v>
       </c>
@@ -39608,8 +39689,11 @@
       <c r="E1121">
         <v>71</v>
       </c>
-    </row>
-    <row r="1122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1122" t="s">
         <v>6</v>
       </c>
@@ -39625,8 +39709,11 @@
       <c r="E1122">
         <v>64</v>
       </c>
-    </row>
-    <row r="1123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1123" t="s">
         <v>6</v>
       </c>
@@ -39642,8 +39729,11 @@
       <c r="E1123">
         <v>99</v>
       </c>
-    </row>
-    <row r="1124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1124" t="s">
         <v>6</v>
       </c>
@@ -39659,8 +39749,11 @@
       <c r="E1124">
         <v>92</v>
       </c>
-    </row>
-    <row r="1125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1125" t="s">
         <v>6</v>
       </c>
@@ -39676,8 +39769,11 @@
       <c r="E1125">
         <v>81</v>
       </c>
-    </row>
-    <row r="1126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1126" t="s">
         <v>6</v>
       </c>
@@ -39693,8 +39789,11 @@
       <c r="E1126">
         <v>10</v>
       </c>
-    </row>
-    <row r="1127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1127" t="s">
         <v>6</v>
       </c>
@@ -39710,8 +39809,11 @@
       <c r="E1127">
         <v>98</v>
       </c>
-    </row>
-    <row r="1128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1128" t="s">
         <v>6</v>
       </c>
@@ -39727,8 +39829,11 @@
       <c r="E1128">
         <v>32</v>
       </c>
-    </row>
-    <row r="1129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1129" t="s">
         <v>6</v>
       </c>
@@ -39744,8 +39849,11 @@
       <c r="E1129">
         <v>98</v>
       </c>
-    </row>
-    <row r="1130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1130" t="s">
         <v>6</v>
       </c>
@@ -39761,8 +39869,11 @@
       <c r="E1130">
         <v>73</v>
       </c>
-    </row>
-    <row r="1131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1131" t="s">
         <v>6</v>
       </c>
@@ -39778,8 +39889,11 @@
       <c r="E1131">
         <v>15</v>
       </c>
-    </row>
-    <row r="1132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1132" t="s">
         <v>6</v>
       </c>
@@ -39795,8 +39909,11 @@
       <c r="E1132">
         <v>86</v>
       </c>
-    </row>
-    <row r="1133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1133" t="s">
         <v>6</v>
       </c>
@@ -39812,8 +39929,11 @@
       <c r="E1133">
         <v>33</v>
       </c>
-    </row>
-    <row r="1134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1134" t="s">
         <v>6</v>
       </c>
@@ -39829,8 +39949,11 @@
       <c r="E1134">
         <v>38</v>
       </c>
-    </row>
-    <row r="1135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1135" t="s">
         <v>6</v>
       </c>
@@ -39846,8 +39969,11 @@
       <c r="E1135">
         <v>71</v>
       </c>
-    </row>
-    <row r="1136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1136" t="s">
         <v>6</v>
       </c>
@@ -39863,8 +39989,11 @@
       <c r="E1136">
         <v>83</v>
       </c>
-    </row>
-    <row r="1137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1137" t="s">
         <v>6</v>
       </c>
@@ -39880,8 +40009,11 @@
       <c r="E1137">
         <v>84</v>
       </c>
-    </row>
-    <row r="1138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1138" t="s">
         <v>6</v>
       </c>
@@ -39897,8 +40029,11 @@
       <c r="E1138">
         <v>30</v>
       </c>
-    </row>
-    <row r="1139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1139" t="s">
         <v>6</v>
       </c>
@@ -39914,8 +40049,11 @@
       <c r="E1139">
         <v>18</v>
       </c>
-    </row>
-    <row r="1140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1140" t="s">
         <v>6</v>
       </c>
@@ -39931,8 +40069,11 @@
       <c r="E1140">
         <v>19</v>
       </c>
-    </row>
-    <row r="1141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1141" t="s">
         <v>6</v>
       </c>
@@ -39948,8 +40089,11 @@
       <c r="E1141">
         <v>60</v>
       </c>
-    </row>
-    <row r="1142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1142" t="s">
         <v>6</v>
       </c>
@@ -39965,8 +40109,11 @@
       <c r="E1142">
         <v>71</v>
       </c>
-    </row>
-    <row r="1143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1143" t="s">
         <v>6</v>
       </c>
@@ -39982,8 +40129,11 @@
       <c r="E1143">
         <v>15</v>
       </c>
-    </row>
-    <row r="1144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1144" t="s">
         <v>6</v>
       </c>
@@ -39999,8 +40149,11 @@
       <c r="E1144">
         <v>88</v>
       </c>
-    </row>
-    <row r="1145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1145" t="s">
         <v>6</v>
       </c>
@@ -40016,8 +40169,11 @@
       <c r="E1145">
         <v>85</v>
       </c>
-    </row>
-    <row r="1146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1146" t="s">
         <v>6</v>
       </c>
@@ -40033,8 +40189,11 @@
       <c r="E1146">
         <v>23</v>
       </c>
-    </row>
-    <row r="1147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1147" t="s">
         <v>6</v>
       </c>
@@ -40050,8 +40209,11 @@
       <c r="E1147">
         <v>31</v>
       </c>
-    </row>
-    <row r="1148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1148" t="s">
         <v>6</v>
       </c>
@@ -40067,8 +40229,11 @@
       <c r="E1148">
         <v>2</v>
       </c>
-    </row>
-    <row r="1149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1149" t="s">
         <v>6</v>
       </c>
@@ -40084,8 +40249,11 @@
       <c r="E1149">
         <v>86</v>
       </c>
-    </row>
-    <row r="1150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1150" t="s">
         <v>6</v>
       </c>
@@ -40101,8 +40269,11 @@
       <c r="E1150">
         <v>65</v>
       </c>
-    </row>
-    <row r="1151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1151" t="s">
         <v>6</v>
       </c>
@@ -40118,8 +40289,11 @@
       <c r="E1151">
         <v>95</v>
       </c>
-    </row>
-    <row r="1152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1152" t="s">
         <v>6</v>
       </c>
@@ -40135,8 +40309,11 @@
       <c r="E1152">
         <v>69</v>
       </c>
-    </row>
-    <row r="1153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1153" t="s">
         <v>6</v>
       </c>
@@ -40152,8 +40329,11 @@
       <c r="E1153">
         <v>74</v>
       </c>
-    </row>
-    <row r="1154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1154" t="s">
         <v>6</v>
       </c>
@@ -40169,8 +40349,11 @@
       <c r="E1154">
         <v>14</v>
       </c>
-    </row>
-    <row r="1155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1155" t="s">
         <v>6</v>
       </c>
@@ -40186,8 +40369,11 @@
       <c r="E1155">
         <v>55</v>
       </c>
-    </row>
-    <row r="1156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1156" t="s">
         <v>6</v>
       </c>
@@ -40203,8 +40389,11 @@
       <c r="E1156">
         <v>75</v>
       </c>
-    </row>
-    <row r="1157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1157" t="s">
         <v>6</v>
       </c>
@@ -40220,8 +40409,11 @@
       <c r="E1157">
         <v>62</v>
       </c>
-    </row>
-    <row r="1158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1158" t="s">
         <v>6</v>
       </c>
@@ -40237,8 +40429,11 @@
       <c r="E1158">
         <v>85</v>
       </c>
-    </row>
-    <row r="1159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1159" t="s">
         <v>6</v>
       </c>
@@ -40254,8 +40449,11 @@
       <c r="E1159">
         <v>81</v>
       </c>
-    </row>
-    <row r="1160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1160" t="s">
         <v>6</v>
       </c>
@@ -40271,8 +40469,11 @@
       <c r="E1160">
         <v>6</v>
       </c>
-    </row>
-    <row r="1161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1161" t="s">
         <v>6</v>
       </c>
@@ -40288,8 +40489,11 @@
       <c r="E1161">
         <v>25</v>
       </c>
-    </row>
-    <row r="1162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1162" t="s">
         <v>6</v>
       </c>
@@ -40305,8 +40509,11 @@
       <c r="E1162">
         <v>74</v>
       </c>
-    </row>
-    <row r="1163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1163" t="s">
         <v>6</v>
       </c>
@@ -40322,8 +40529,11 @@
       <c r="E1163">
         <v>90</v>
       </c>
-    </row>
-    <row r="1164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1164" t="s">
         <v>6</v>
       </c>
@@ -40339,8 +40549,11 @@
       <c r="E1164">
         <v>35</v>
       </c>
-    </row>
-    <row r="1165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1165" t="s">
         <v>6</v>
       </c>
@@ -40356,8 +40569,11 @@
       <c r="E1165">
         <v>17</v>
       </c>
-    </row>
-    <row r="1166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1166" t="s">
         <v>6</v>
       </c>
@@ -40373,8 +40589,11 @@
       <c r="E1166">
         <v>69</v>
       </c>
-    </row>
-    <row r="1167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1167" t="s">
         <v>6</v>
       </c>
@@ -40390,8 +40609,11 @@
       <c r="E1167">
         <v>93</v>
       </c>
-    </row>
-    <row r="1168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1168" t="s">
         <v>6</v>
       </c>
@@ -40407,8 +40629,11 @@
       <c r="E1168">
         <v>75</v>
       </c>
-    </row>
-    <row r="1169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1169" t="s">
         <v>6</v>
       </c>
@@ -40424,8 +40649,11 @@
       <c r="E1169">
         <v>28</v>
       </c>
-    </row>
-    <row r="1170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1170" t="s">
         <v>6</v>
       </c>
@@ -40441,8 +40669,11 @@
       <c r="E1170">
         <v>79</v>
       </c>
-    </row>
-    <row r="1171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1171" t="s">
         <v>6</v>
       </c>
@@ -40458,8 +40689,11 @@
       <c r="E1171">
         <v>28</v>
       </c>
-    </row>
-    <row r="1172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1172" t="s">
         <v>6</v>
       </c>
@@ -40475,8 +40709,11 @@
       <c r="E1172">
         <v>95</v>
       </c>
-    </row>
-    <row r="1173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1173" t="s">
         <v>6</v>
       </c>
@@ -40492,8 +40729,11 @@
       <c r="E1173">
         <v>82</v>
       </c>
-    </row>
-    <row r="1174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1174" t="s">
         <v>6</v>
       </c>
@@ -40509,8 +40749,11 @@
       <c r="E1174">
         <v>22</v>
       </c>
-    </row>
-    <row r="1175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1175" t="s">
         <v>6</v>
       </c>
@@ -40526,8 +40769,11 @@
       <c r="E1175">
         <v>100</v>
       </c>
-    </row>
-    <row r="1176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1176" t="s">
         <v>6</v>
       </c>
@@ -40543,8 +40789,11 @@
       <c r="E1176">
         <v>31</v>
       </c>
-    </row>
-    <row r="1177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1177" t="s">
         <v>6</v>
       </c>
@@ -40560,8 +40809,11 @@
       <c r="E1177">
         <v>12</v>
       </c>
-    </row>
-    <row r="1178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1178" t="s">
         <v>6</v>
       </c>
@@ -40577,8 +40829,11 @@
       <c r="E1178">
         <v>14</v>
       </c>
-    </row>
-    <row r="1179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1178">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1179" t="s">
         <v>6</v>
       </c>
@@ -40594,8 +40849,11 @@
       <c r="E1179">
         <v>51</v>
       </c>
-    </row>
-    <row r="1180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1180" t="s">
         <v>6</v>
       </c>
@@ -40611,8 +40869,11 @@
       <c r="E1180">
         <v>67</v>
       </c>
-    </row>
-    <row r="1181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1181" t="s">
         <v>6</v>
       </c>
@@ -40628,8 +40889,11 @@
       <c r="E1181">
         <v>20</v>
       </c>
-    </row>
-    <row r="1182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1182" t="s">
         <v>6</v>
       </c>
@@ -40645,8 +40909,11 @@
       <c r="E1182">
         <v>7</v>
       </c>
-    </row>
-    <row r="1183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1183" t="s">
         <v>6</v>
       </c>
@@ -40662,8 +40929,11 @@
       <c r="E1183">
         <v>70</v>
       </c>
-    </row>
-    <row r="1184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1184" t="s">
         <v>6</v>
       </c>
@@ -40679,6 +40949,9 @@
       <c r="E1184">
         <v>40</v>
       </c>
+      <c r="F1184">
+        <v>1</v>
+      </c>
     </row>
     <row r="1185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1185" t="s">
@@ -40696,6 +40969,9 @@
       <c r="E1185">
         <v>95</v>
       </c>
+      <c r="F1185">
+        <v>1</v>
+      </c>
     </row>
     <row r="1186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1186" t="s">
@@ -40713,6 +40989,9 @@
       <c r="E1186">
         <v>87</v>
       </c>
+      <c r="F1186">
+        <v>1</v>
+      </c>
     </row>
     <row r="1187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1187" t="s">
@@ -40730,6 +41009,9 @@
       <c r="E1187">
         <v>70</v>
       </c>
+      <c r="F1187">
+        <v>2</v>
+      </c>
     </row>
     <row r="1188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1188" t="s">
@@ -40747,6 +41029,9 @@
       <c r="E1188">
         <v>13</v>
       </c>
+      <c r="F1188">
+        <v>0</v>
+      </c>
     </row>
     <row r="1189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1189" t="s">
@@ -40764,6 +41049,9 @@
       <c r="E1189">
         <v>64</v>
       </c>
+      <c r="F1189">
+        <v>1</v>
+      </c>
     </row>
     <row r="1190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1190" t="s">
@@ -40781,6 +41069,9 @@
       <c r="E1190">
         <v>38</v>
       </c>
+      <c r="F1190">
+        <v>1</v>
+      </c>
     </row>
     <row r="1191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1191" t="s">
@@ -40798,6 +41089,9 @@
       <c r="E1191">
         <v>86</v>
       </c>
+      <c r="F1191">
+        <v>2</v>
+      </c>
     </row>
     <row r="1192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1192" t="s">
@@ -40815,6 +41109,9 @@
       <c r="E1192">
         <v>92</v>
       </c>
+      <c r="F1192">
+        <v>1</v>
+      </c>
     </row>
     <row r="1193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1193" t="s">
@@ -40832,6 +41129,9 @@
       <c r="E1193">
         <v>74</v>
       </c>
+      <c r="F1193">
+        <v>1</v>
+      </c>
     </row>
     <row r="1194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1194" t="s">
@@ -40849,6 +41149,9 @@
       <c r="E1194">
         <v>9</v>
       </c>
+      <c r="F1194">
+        <v>1</v>
+      </c>
     </row>
     <row r="1195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1195" t="s">
@@ -40866,6 +41169,9 @@
       <c r="E1195">
         <v>37</v>
       </c>
+      <c r="F1195">
+        <v>1</v>
+      </c>
     </row>
     <row r="1196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1196" t="s">
@@ -40883,6 +41189,9 @@
       <c r="E1196">
         <v>33</v>
       </c>
+      <c r="F1196">
+        <v>0</v>
+      </c>
     </row>
     <row r="1197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1197" t="s">
@@ -40900,6 +41209,9 @@
       <c r="E1197">
         <v>16</v>
       </c>
+      <c r="F1197">
+        <v>1</v>
+      </c>
     </row>
     <row r="1198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1198" t="s">
@@ -40917,6 +41229,9 @@
       <c r="E1198">
         <v>85</v>
       </c>
+      <c r="F1198">
+        <v>1</v>
+      </c>
     </row>
     <row r="1199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1199" t="s">
@@ -40933,6 +41248,9 @@
       </c>
       <c r="E1199">
         <v>66</v>
+      </c>
+      <c r="F1199">
+        <v>0</v>
       </c>
     </row>
     <row r="1200" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
preenchimento da coluna Target
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b866b217d0e5359/Área de Trabalho/Insper/2o semestre/Ciência dos Dados/Projeto 1/22-2b-cd-p1-grupo_joaoogp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{6AFCFE07-6B38-4DB7-9263-61A542C365A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC0251BC-59D5-40B6-850B-1F0323FF5BD1}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{6AFCFE07-6B38-4DB7-9263-61A542C365A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDF7A654-B8AC-4640-A7F8-458DAE48C3E8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18115,8 +18115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1076" workbookViewId="0">
-      <selection activeCell="O1094" sqref="O1094"/>
+    <sheetView tabSelected="1" topLeftCell="A951" workbookViewId="0">
+      <selection activeCell="I954" sqref="I954"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36600,7 +36600,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="945" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="945" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A945" t="s">
         <v>6</v>
       </c>
@@ -36617,7 +36617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="946" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="946" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A946" t="s">
         <v>6</v>
       </c>
@@ -36634,7 +36634,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="947" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="947" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A947" t="s">
         <v>6</v>
       </c>
@@ -36651,7 +36651,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="948" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="948" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A948" t="s">
         <v>6</v>
       </c>
@@ -36668,7 +36668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="949" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="949" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A949" t="s">
         <v>6</v>
       </c>
@@ -36685,7 +36685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="950" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="950" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A950" t="s">
         <v>6</v>
       </c>
@@ -36702,7 +36702,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="951" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="951" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A951" t="s">
         <v>6</v>
       </c>
@@ -36718,8 +36718,11 @@
       <c r="E951">
         <v>25</v>
       </c>
-    </row>
-    <row r="952" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F951">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="952" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A952" t="s">
         <v>6</v>
       </c>
@@ -36735,8 +36738,11 @@
       <c r="E952">
         <v>48</v>
       </c>
-    </row>
-    <row r="953" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F952">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="953" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A953" t="s">
         <v>6</v>
       </c>
@@ -36752,8 +36758,11 @@
       <c r="E953">
         <v>62</v>
       </c>
-    </row>
-    <row r="954" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F953">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="954" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A954" t="s">
         <v>6</v>
       </c>
@@ -36769,8 +36778,11 @@
       <c r="E954">
         <v>18</v>
       </c>
-    </row>
-    <row r="955" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F954">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="955" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A955" t="s">
         <v>6</v>
       </c>
@@ -36786,8 +36798,11 @@
       <c r="E955">
         <v>13</v>
       </c>
-    </row>
-    <row r="956" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F955">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="956" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A956" t="s">
         <v>6</v>
       </c>
@@ -36803,8 +36818,11 @@
       <c r="E956">
         <v>82</v>
       </c>
-    </row>
-    <row r="957" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F956">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="957" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A957" t="s">
         <v>6</v>
       </c>
@@ -36820,8 +36838,11 @@
       <c r="E957">
         <v>4</v>
       </c>
-    </row>
-    <row r="958" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F957">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="958" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A958" t="s">
         <v>6</v>
       </c>
@@ -36837,8 +36858,11 @@
       <c r="E958">
         <v>8</v>
       </c>
-    </row>
-    <row r="959" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F958">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="959" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A959" t="s">
         <v>6</v>
       </c>
@@ -36854,8 +36878,11 @@
       <c r="E959">
         <v>9</v>
       </c>
-    </row>
-    <row r="960" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F959">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="960" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A960" t="s">
         <v>6</v>
       </c>
@@ -36871,8 +36898,11 @@
       <c r="E960">
         <v>79</v>
       </c>
-    </row>
-    <row r="961" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F960">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="961" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A961" t="s">
         <v>6</v>
       </c>
@@ -36888,8 +36918,11 @@
       <c r="E961">
         <v>28</v>
       </c>
-    </row>
-    <row r="962" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F961">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="962" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A962" t="s">
         <v>6</v>
       </c>
@@ -36905,8 +36938,11 @@
       <c r="E962">
         <v>69</v>
       </c>
-    </row>
-    <row r="963" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F962">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="963" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A963" t="s">
         <v>6</v>
       </c>
@@ -36922,8 +36958,11 @@
       <c r="E963">
         <v>92</v>
       </c>
-    </row>
-    <row r="964" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F963">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="964" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A964" t="s">
         <v>6</v>
       </c>
@@ -36939,8 +36978,11 @@
       <c r="E964">
         <v>68</v>
       </c>
-    </row>
-    <row r="965" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F964">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="965" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A965" t="s">
         <v>6</v>
       </c>
@@ -36956,8 +36998,11 @@
       <c r="E965">
         <v>77</v>
       </c>
-    </row>
-    <row r="966" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F965">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="966" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A966" t="s">
         <v>6</v>
       </c>
@@ -36973,8 +37018,11 @@
       <c r="E966">
         <v>47</v>
       </c>
-    </row>
-    <row r="967" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F966">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="967" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A967" t="s">
         <v>6</v>
       </c>
@@ -36990,8 +37038,11 @@
       <c r="E967">
         <v>13</v>
       </c>
-    </row>
-    <row r="968" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F967">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="968" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A968" t="s">
         <v>6</v>
       </c>
@@ -37007,8 +37058,11 @@
       <c r="E968">
         <v>11</v>
       </c>
-    </row>
-    <row r="969" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F968">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="969" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A969" t="s">
         <v>6</v>
       </c>
@@ -37024,8 +37078,11 @@
       <c r="E969">
         <v>25</v>
       </c>
-    </row>
-    <row r="970" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F969">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="970" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A970" t="s">
         <v>6</v>
       </c>
@@ -37041,8 +37098,11 @@
       <c r="E970">
         <v>81</v>
       </c>
-    </row>
-    <row r="971" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F970">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="971" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A971" t="s">
         <v>6</v>
       </c>
@@ -37058,8 +37118,11 @@
       <c r="E971">
         <v>5</v>
       </c>
-    </row>
-    <row r="972" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F971">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="972" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A972" t="s">
         <v>6</v>
       </c>
@@ -37075,8 +37138,11 @@
       <c r="E972">
         <v>8</v>
       </c>
-    </row>
-    <row r="973" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F972">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="973" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A973" t="s">
         <v>6</v>
       </c>
@@ -37092,8 +37158,11 @@
       <c r="E973">
         <v>45</v>
       </c>
-    </row>
-    <row r="974" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F973">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="974" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A974" t="s">
         <v>6</v>
       </c>
@@ -37109,8 +37178,11 @@
       <c r="E974">
         <v>31</v>
       </c>
-    </row>
-    <row r="975" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F974">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="975" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A975" t="s">
         <v>6</v>
       </c>
@@ -37126,8 +37198,11 @@
       <c r="E975">
         <v>87</v>
       </c>
-    </row>
-    <row r="976" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F975">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="976" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A976" t="s">
         <v>6</v>
       </c>
@@ -37143,8 +37218,11 @@
       <c r="E976">
         <v>86</v>
       </c>
-    </row>
-    <row r="977" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F976">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="977" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A977" t="s">
         <v>6</v>
       </c>
@@ -37160,8 +37238,11 @@
       <c r="E977">
         <v>74</v>
       </c>
-    </row>
-    <row r="978" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F977">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="978" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A978" t="s">
         <v>6</v>
       </c>
@@ -37177,8 +37258,11 @@
       <c r="E978">
         <v>36</v>
       </c>
-    </row>
-    <row r="979" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F978">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="979" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A979" t="s">
         <v>6</v>
       </c>
@@ -37194,8 +37278,11 @@
       <c r="E979">
         <v>54</v>
       </c>
-    </row>
-    <row r="980" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F979">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="980" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A980" t="s">
         <v>6</v>
       </c>
@@ -37211,8 +37298,11 @@
       <c r="E980">
         <v>27</v>
       </c>
-    </row>
-    <row r="981" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F980">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="981" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A981" t="s">
         <v>6</v>
       </c>
@@ -37228,8 +37318,11 @@
       <c r="E981">
         <v>62</v>
       </c>
-    </row>
-    <row r="982" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F981">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="982" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A982" t="s">
         <v>6</v>
       </c>
@@ -37245,8 +37338,11 @@
       <c r="E982">
         <v>100</v>
       </c>
-    </row>
-    <row r="983" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F982">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="983" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A983" t="s">
         <v>6</v>
       </c>
@@ -37262,8 +37358,11 @@
       <c r="E983">
         <v>60</v>
       </c>
-    </row>
-    <row r="984" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F983">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="984" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A984" t="s">
         <v>6</v>
       </c>
@@ -37279,8 +37378,11 @@
       <c r="E984">
         <v>44</v>
       </c>
-    </row>
-    <row r="985" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F984">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="985" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A985" t="s">
         <v>6</v>
       </c>
@@ -37296,8 +37398,11 @@
       <c r="E985">
         <v>40</v>
       </c>
-    </row>
-    <row r="986" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F985">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="986" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A986" t="s">
         <v>6</v>
       </c>
@@ -37313,8 +37418,11 @@
       <c r="E986">
         <v>37</v>
       </c>
-    </row>
-    <row r="987" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F986">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="987" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A987" t="s">
         <v>6</v>
       </c>
@@ -37330,8 +37438,11 @@
       <c r="E987">
         <v>94</v>
       </c>
-    </row>
-    <row r="988" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F987">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="988" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A988" t="s">
         <v>6</v>
       </c>
@@ -37347,8 +37458,11 @@
       <c r="E988">
         <v>58</v>
       </c>
-    </row>
-    <row r="989" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F988">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="989" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A989" t="s">
         <v>6</v>
       </c>
@@ -37364,8 +37478,11 @@
       <c r="E989">
         <v>18</v>
       </c>
-    </row>
-    <row r="990" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F989">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="990" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A990" t="s">
         <v>6</v>
       </c>
@@ -37381,8 +37498,11 @@
       <c r="E990">
         <v>4</v>
       </c>
-    </row>
-    <row r="991" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F990">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="991" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A991" t="s">
         <v>6</v>
       </c>
@@ -37398,8 +37518,11 @@
       <c r="E991">
         <v>50</v>
       </c>
-    </row>
-    <row r="992" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F991">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="992" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A992" t="s">
         <v>6</v>
       </c>
@@ -37415,8 +37538,11 @@
       <c r="E992">
         <v>95</v>
       </c>
-    </row>
-    <row r="993" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F992">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="993" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A993" t="s">
         <v>6</v>
       </c>
@@ -37432,8 +37558,11 @@
       <c r="E993">
         <v>28</v>
       </c>
-    </row>
-    <row r="994" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F993">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="994" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A994" t="s">
         <v>6</v>
       </c>
@@ -37449,8 +37578,11 @@
       <c r="E994">
         <v>3</v>
       </c>
-    </row>
-    <row r="995" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F994">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="995" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A995" t="s">
         <v>6</v>
       </c>
@@ -37466,8 +37598,11 @@
       <c r="E995">
         <v>2</v>
       </c>
-    </row>
-    <row r="996" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F995">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="996" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A996" t="s">
         <v>6</v>
       </c>
@@ -37483,8 +37618,11 @@
       <c r="E996">
         <v>69</v>
       </c>
-    </row>
-    <row r="997" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F996">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="997" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A997" t="s">
         <v>6</v>
       </c>
@@ -37500,8 +37638,11 @@
       <c r="E997">
         <v>16</v>
       </c>
-    </row>
-    <row r="998" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F997">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="998" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A998" t="s">
         <v>6</v>
       </c>
@@ -37517,8 +37658,11 @@
       <c r="E998">
         <v>79</v>
       </c>
-    </row>
-    <row r="999" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F998">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="999" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A999" t="s">
         <v>6</v>
       </c>
@@ -37534,8 +37678,11 @@
       <c r="E999">
         <v>34</v>
       </c>
-    </row>
-    <row r="1000" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F999">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1000" t="s">
         <v>6</v>
       </c>
@@ -37551,8 +37698,11 @@
       <c r="E1000">
         <v>88</v>
       </c>
-    </row>
-    <row r="1001" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1000">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1001" t="s">
         <v>6</v>
       </c>
@@ -37568,8 +37718,11 @@
       <c r="E1001">
         <v>67</v>
       </c>
-    </row>
-    <row r="1002" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1001">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1002" t="s">
         <v>6</v>
       </c>
@@ -37585,8 +37738,11 @@
       <c r="E1002">
         <v>38</v>
       </c>
-    </row>
-    <row r="1003" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1002">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1003" t="s">
         <v>6</v>
       </c>
@@ -37602,8 +37758,11 @@
       <c r="E1003">
         <v>7</v>
       </c>
-    </row>
-    <row r="1004" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1003">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1004" t="s">
         <v>6</v>
       </c>
@@ -37619,8 +37778,11 @@
       <c r="E1004">
         <v>82</v>
       </c>
-    </row>
-    <row r="1005" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1004">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1005" t="s">
         <v>6</v>
       </c>
@@ -37636,8 +37798,11 @@
       <c r="E1005">
         <v>94</v>
       </c>
-    </row>
-    <row r="1006" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1005">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1006" t="s">
         <v>6</v>
       </c>
@@ -37653,8 +37818,11 @@
       <c r="E1006">
         <v>95</v>
       </c>
-    </row>
-    <row r="1007" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1006">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1007" t="s">
         <v>6</v>
       </c>
@@ -37670,8 +37838,11 @@
       <c r="E1007">
         <v>14</v>
       </c>
-    </row>
-    <row r="1008" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1007">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1008" t="s">
         <v>6</v>
       </c>
@@ -37687,8 +37858,11 @@
       <c r="E1008">
         <v>4</v>
       </c>
-    </row>
-    <row r="1009" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1008">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1009" t="s">
         <v>6</v>
       </c>
@@ -37704,8 +37878,11 @@
       <c r="E1009">
         <v>67</v>
       </c>
-    </row>
-    <row r="1010" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1009">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1010" t="s">
         <v>6</v>
       </c>
@@ -37721,8 +37898,11 @@
       <c r="E1010">
         <v>1</v>
       </c>
-    </row>
-    <row r="1011" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1010">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1011" t="s">
         <v>6</v>
       </c>
@@ -37738,8 +37918,11 @@
       <c r="E1011">
         <v>43</v>
       </c>
-    </row>
-    <row r="1012" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1011">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1012" t="s">
         <v>6</v>
       </c>
@@ -37755,8 +37938,11 @@
       <c r="E1012">
         <v>100</v>
       </c>
-    </row>
-    <row r="1013" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1012">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1013" t="s">
         <v>6</v>
       </c>
@@ -37772,8 +37958,11 @@
       <c r="E1013">
         <v>19</v>
       </c>
-    </row>
-    <row r="1014" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1013">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1014" t="s">
         <v>6</v>
       </c>
@@ -37789,8 +37978,11 @@
       <c r="E1014">
         <v>46</v>
       </c>
-    </row>
-    <row r="1015" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1014">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1015" t="s">
         <v>6</v>
       </c>
@@ -37806,8 +37998,11 @@
       <c r="E1015">
         <v>39</v>
       </c>
-    </row>
-    <row r="1016" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1015">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1016" t="s">
         <v>6</v>
       </c>
@@ -37823,8 +38018,11 @@
       <c r="E1016">
         <v>10</v>
       </c>
-    </row>
-    <row r="1017" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1016">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1017" t="s">
         <v>6</v>
       </c>
@@ -37840,8 +38038,11 @@
       <c r="E1017">
         <v>11</v>
       </c>
-    </row>
-    <row r="1018" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1017">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1018" t="s">
         <v>6</v>
       </c>
@@ -37857,8 +38058,11 @@
       <c r="E1018">
         <v>11</v>
       </c>
-    </row>
-    <row r="1019" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1018">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1019" t="s">
         <v>6</v>
       </c>
@@ -37874,8 +38078,11 @@
       <c r="E1019">
         <v>15</v>
       </c>
-    </row>
-    <row r="1020" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1019">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1020" t="s">
         <v>6</v>
       </c>
@@ -37891,8 +38098,11 @@
       <c r="E1020">
         <v>81</v>
       </c>
-    </row>
-    <row r="1021" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1020">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1021" t="s">
         <v>6</v>
       </c>
@@ -37908,8 +38118,11 @@
       <c r="E1021">
         <v>63</v>
       </c>
-    </row>
-    <row r="1022" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1021">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1022" t="s">
         <v>6</v>
       </c>
@@ -37925,8 +38138,11 @@
       <c r="E1022">
         <v>60</v>
       </c>
-    </row>
-    <row r="1023" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1022">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1023" t="s">
         <v>6</v>
       </c>
@@ -37942,8 +38158,11 @@
       <c r="E1023">
         <v>9</v>
       </c>
-    </row>
-    <row r="1024" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1023">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1024" t="s">
         <v>6</v>
       </c>
@@ -37959,8 +38178,11 @@
       <c r="E1024">
         <v>24</v>
       </c>
-    </row>
-    <row r="1025" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1024">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1025" t="s">
         <v>6</v>
       </c>
@@ -37976,8 +38198,11 @@
       <c r="E1025">
         <v>86</v>
       </c>
-    </row>
-    <row r="1026" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1025">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1026" t="s">
         <v>6</v>
       </c>
@@ -37993,8 +38218,11 @@
       <c r="E1026">
         <v>19</v>
       </c>
-    </row>
-    <row r="1027" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1026">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1027" t="s">
         <v>6</v>
       </c>
@@ -38010,8 +38238,11 @@
       <c r="E1027">
         <v>84</v>
       </c>
-    </row>
-    <row r="1028" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1027">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1028" t="s">
         <v>6</v>
       </c>
@@ -38027,8 +38258,11 @@
       <c r="E1028">
         <v>33</v>
       </c>
-    </row>
-    <row r="1029" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1028">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1029" t="s">
         <v>6</v>
       </c>
@@ -38044,8 +38278,11 @@
       <c r="E1029">
         <v>45</v>
       </c>
-    </row>
-    <row r="1030" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1029">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1030" t="s">
         <v>6</v>
       </c>
@@ -38061,8 +38298,11 @@
       <c r="E1030">
         <v>77</v>
       </c>
-    </row>
-    <row r="1031" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1030">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1031" t="s">
         <v>6</v>
       </c>
@@ -38078,8 +38318,11 @@
       <c r="E1031">
         <v>31</v>
       </c>
-    </row>
-    <row r="1032" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1031">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1032" t="s">
         <v>6</v>
       </c>
@@ -38095,8 +38338,11 @@
       <c r="E1032">
         <v>66</v>
       </c>
-    </row>
-    <row r="1033" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1032">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1033" t="s">
         <v>6</v>
       </c>
@@ -38112,8 +38358,11 @@
       <c r="E1033">
         <v>3</v>
       </c>
-    </row>
-    <row r="1034" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1033">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1034" t="s">
         <v>6</v>
       </c>
@@ -38129,8 +38378,11 @@
       <c r="E1034">
         <v>4</v>
       </c>
-    </row>
-    <row r="1035" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1034">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1035" t="s">
         <v>6</v>
       </c>
@@ -38146,8 +38398,11 @@
       <c r="E1035">
         <v>89</v>
       </c>
-    </row>
-    <row r="1036" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1035">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1036" t="s">
         <v>6</v>
       </c>
@@ -38163,8 +38418,11 @@
       <c r="E1036">
         <v>83</v>
       </c>
-    </row>
-    <row r="1037" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1036">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1037" t="s">
         <v>6</v>
       </c>
@@ -38180,8 +38438,11 @@
       <c r="E1037">
         <v>36</v>
       </c>
-    </row>
-    <row r="1038" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1037">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1038" t="s">
         <v>6</v>
       </c>
@@ -38197,8 +38458,11 @@
       <c r="E1038">
         <v>92</v>
       </c>
-    </row>
-    <row r="1039" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1038">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1039" t="s">
         <v>6</v>
       </c>
@@ -38214,8 +38478,11 @@
       <c r="E1039">
         <v>40</v>
       </c>
-    </row>
-    <row r="1040" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1039">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1040" t="s">
         <v>6</v>
       </c>
@@ -38231,8 +38498,11 @@
       <c r="E1040">
         <v>78</v>
       </c>
-    </row>
-    <row r="1041" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1040">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1041" t="s">
         <v>6</v>
       </c>
@@ -38248,8 +38518,11 @@
       <c r="E1041">
         <v>5</v>
       </c>
-    </row>
-    <row r="1042" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1041">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1042" t="s">
         <v>6</v>
       </c>
@@ -38265,8 +38538,11 @@
       <c r="E1042">
         <v>44</v>
       </c>
-    </row>
-    <row r="1043" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1042">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1043" t="s">
         <v>6</v>
       </c>
@@ -38282,8 +38558,11 @@
       <c r="E1043">
         <v>47</v>
       </c>
-    </row>
-    <row r="1044" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1043">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1044" t="s">
         <v>6</v>
       </c>
@@ -38299,8 +38578,11 @@
       <c r="E1044">
         <v>30</v>
       </c>
-    </row>
-    <row r="1045" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1044">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1045" t="s">
         <v>6</v>
       </c>
@@ -38316,8 +38598,11 @@
       <c r="E1045">
         <v>99</v>
       </c>
-    </row>
-    <row r="1046" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1045">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1046" t="s">
         <v>6</v>
       </c>
@@ -38333,8 +38618,11 @@
       <c r="E1046">
         <v>12</v>
       </c>
-    </row>
-    <row r="1047" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1046">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1047" t="s">
         <v>6</v>
       </c>
@@ -38350,8 +38638,11 @@
       <c r="E1047">
         <v>98</v>
       </c>
-    </row>
-    <row r="1048" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1047">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1048" t="s">
         <v>6</v>
       </c>
@@ -38367,8 +38658,11 @@
       <c r="E1048">
         <v>51</v>
       </c>
-    </row>
-    <row r="1049" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1048">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1049" t="s">
         <v>6</v>
       </c>
@@ -38384,8 +38678,11 @@
       <c r="E1049">
         <v>49</v>
       </c>
-    </row>
-    <row r="1050" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1049">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1050" t="s">
         <v>6</v>
       </c>
@@ -38401,8 +38698,11 @@
       <c r="E1050">
         <v>24</v>
       </c>
-    </row>
-    <row r="1051" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1050">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1051" t="s">
         <v>6</v>
       </c>
@@ -38418,8 +38718,11 @@
       <c r="E1051">
         <v>10</v>
       </c>
-    </row>
-    <row r="1052" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1051">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1052" t="s">
         <v>6</v>
       </c>
@@ -38435,8 +38738,11 @@
       <c r="E1052">
         <v>94</v>
       </c>
-    </row>
-    <row r="1053" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1052">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1053" t="s">
         <v>6</v>
       </c>
@@ -38452,8 +38758,11 @@
       <c r="E1053">
         <v>49</v>
       </c>
-    </row>
-    <row r="1054" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1053">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1054" t="s">
         <v>6</v>
       </c>
@@ -38469,8 +38778,11 @@
       <c r="E1054">
         <v>8</v>
       </c>
-    </row>
-    <row r="1055" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1054">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1055" t="s">
         <v>6</v>
       </c>
@@ -38486,8 +38798,11 @@
       <c r="E1055">
         <v>92</v>
       </c>
-    </row>
-    <row r="1056" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1055">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1056" t="s">
         <v>6</v>
       </c>
@@ -38503,8 +38818,11 @@
       <c r="E1056">
         <v>12</v>
       </c>
-    </row>
-    <row r="1057" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1056">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1057" t="s">
         <v>6</v>
       </c>
@@ -38520,8 +38838,11 @@
       <c r="E1057">
         <v>77</v>
       </c>
-    </row>
-    <row r="1058" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1057">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1058" t="s">
         <v>6</v>
       </c>
@@ -38537,8 +38858,11 @@
       <c r="E1058">
         <v>71</v>
       </c>
-    </row>
-    <row r="1059" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1058">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1059" t="s">
         <v>6</v>
       </c>
@@ -38554,8 +38878,11 @@
       <c r="E1059">
         <v>45</v>
       </c>
-    </row>
-    <row r="1060" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1059">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1060" t="s">
         <v>6</v>
       </c>
@@ -38571,8 +38898,11 @@
       <c r="E1060">
         <v>94</v>
       </c>
-    </row>
-    <row r="1061" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1060">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1061" t="s">
         <v>6</v>
       </c>
@@ -38588,8 +38918,11 @@
       <c r="E1061">
         <v>4</v>
       </c>
-    </row>
-    <row r="1062" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1061">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1062" t="s">
         <v>6</v>
       </c>
@@ -38605,8 +38938,11 @@
       <c r="E1062">
         <v>76</v>
       </c>
-    </row>
-    <row r="1063" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1062">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1063" t="s">
         <v>6</v>
       </c>
@@ -38622,8 +38958,11 @@
       <c r="E1063">
         <v>93</v>
       </c>
-    </row>
-    <row r="1064" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1063">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1064" t="s">
         <v>6</v>
       </c>
@@ -38639,8 +38978,11 @@
       <c r="E1064">
         <v>9</v>
       </c>
-    </row>
-    <row r="1065" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1064">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1065" t="s">
         <v>6</v>
       </c>
@@ -38656,8 +38998,11 @@
       <c r="E1065">
         <v>63</v>
       </c>
-    </row>
-    <row r="1066" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1065">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1066" t="s">
         <v>6</v>
       </c>
@@ -38673,8 +39018,11 @@
       <c r="E1066">
         <v>3</v>
       </c>
-    </row>
-    <row r="1067" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1066">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1067" t="s">
         <v>6</v>
       </c>
@@ -38690,8 +39038,11 @@
       <c r="E1067">
         <v>82</v>
       </c>
-    </row>
-    <row r="1068" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1067">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1068" t="s">
         <v>6</v>
       </c>
@@ -38707,8 +39058,11 @@
       <c r="E1068">
         <v>62</v>
       </c>
-    </row>
-    <row r="1069" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1068">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1069" t="s">
         <v>6</v>
       </c>
@@ -38724,8 +39078,11 @@
       <c r="E1069">
         <v>11</v>
       </c>
-    </row>
-    <row r="1070" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1069">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1070" t="s">
         <v>6</v>
       </c>
@@ -38741,8 +39098,11 @@
       <c r="E1070">
         <v>2</v>
       </c>
-    </row>
-    <row r="1071" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1070">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1071" t="s">
         <v>6</v>
       </c>
@@ -38758,8 +39118,11 @@
       <c r="E1071">
         <v>76</v>
       </c>
-    </row>
-    <row r="1072" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1071">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1072" t="s">
         <v>6</v>
       </c>
@@ -38775,8 +39138,11 @@
       <c r="E1072">
         <v>20</v>
       </c>
-    </row>
-    <row r="1073" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1072">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1073" t="s">
         <v>6</v>
       </c>
@@ -38792,8 +39158,11 @@
       <c r="E1073">
         <v>29</v>
       </c>
-    </row>
-    <row r="1074" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1073">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1074" t="s">
         <v>6</v>
       </c>
@@ -38809,8 +39178,11 @@
       <c r="E1074">
         <v>34</v>
       </c>
-    </row>
-    <row r="1075" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1074">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1075" t="s">
         <v>6</v>
       </c>
@@ -38826,8 +39198,11 @@
       <c r="E1075">
         <v>69</v>
       </c>
-    </row>
-    <row r="1076" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1075">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1076" t="s">
         <v>6</v>
       </c>
@@ -38843,8 +39218,11 @@
       <c r="E1076">
         <v>22</v>
       </c>
-    </row>
-    <row r="1077" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1076">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1077" t="s">
         <v>6</v>
       </c>
@@ -38860,8 +39238,11 @@
       <c r="E1077">
         <v>82</v>
       </c>
-    </row>
-    <row r="1078" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1077">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1078" t="s">
         <v>6</v>
       </c>
@@ -38877,8 +39258,11 @@
       <c r="E1078">
         <v>62</v>
       </c>
-    </row>
-    <row r="1079" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1078">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1079" t="s">
         <v>6</v>
       </c>
@@ -38894,8 +39278,11 @@
       <c r="E1079">
         <v>86</v>
       </c>
-    </row>
-    <row r="1080" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1079">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1080" t="s">
         <v>6</v>
       </c>
@@ -38911,8 +39298,11 @@
       <c r="E1080">
         <v>6</v>
       </c>
-    </row>
-    <row r="1081" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1080">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1081" t="s">
         <v>6</v>
       </c>
@@ -38928,8 +39318,11 @@
       <c r="E1081">
         <v>30</v>
       </c>
-    </row>
-    <row r="1082" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1081">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1082" t="s">
         <v>6</v>
       </c>
@@ -38945,8 +39338,11 @@
       <c r="E1082">
         <v>86</v>
       </c>
-    </row>
-    <row r="1083" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1082">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1083" t="s">
         <v>6</v>
       </c>
@@ -38962,8 +39358,11 @@
       <c r="E1083">
         <v>80</v>
       </c>
-    </row>
-    <row r="1084" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1083">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1084" t="s">
         <v>6</v>
       </c>
@@ -38979,8 +39378,11 @@
       <c r="E1084">
         <v>33</v>
       </c>
-    </row>
-    <row r="1085" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1084">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1085" t="s">
         <v>6</v>
       </c>
@@ -38996,8 +39398,11 @@
       <c r="E1085">
         <v>16</v>
       </c>
-    </row>
-    <row r="1086" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1085">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1086" t="s">
         <v>6</v>
       </c>
@@ -39013,8 +39418,11 @@
       <c r="E1086">
         <v>83</v>
       </c>
-    </row>
-    <row r="1087" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1086">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1087" t="s">
         <v>6</v>
       </c>
@@ -39030,8 +39438,11 @@
       <c r="E1087">
         <v>66</v>
       </c>
-    </row>
-    <row r="1088" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1087">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1088" t="s">
         <v>6</v>
       </c>
@@ -39047,6 +39458,9 @@
       <c r="E1088">
         <v>97</v>
       </c>
+      <c r="F1088">
+        <v>0</v>
+      </c>
     </row>
     <row r="1089" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1089" t="s">
@@ -39064,6 +39478,9 @@
       <c r="E1089">
         <v>26</v>
       </c>
+      <c r="F1089">
+        <v>1</v>
+      </c>
     </row>
     <row r="1090" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1090" t="s">
@@ -39081,6 +39498,9 @@
       <c r="E1090">
         <v>57</v>
       </c>
+      <c r="F1090">
+        <v>1</v>
+      </c>
     </row>
     <row r="1091" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1091" t="s">
@@ -39098,6 +39518,9 @@
       <c r="E1091">
         <v>48</v>
       </c>
+      <c r="F1091">
+        <v>0</v>
+      </c>
     </row>
     <row r="1092" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1092" t="s">
@@ -39115,6 +39538,9 @@
       <c r="E1092">
         <v>25</v>
       </c>
+      <c r="F1092">
+        <v>2</v>
+      </c>
     </row>
     <row r="1093" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1093" t="s">
@@ -39131,6 +39557,9 @@
       </c>
       <c r="E1093">
         <v>36</v>
+      </c>
+      <c r="F1093">
+        <v>1</v>
       </c>
     </row>
     <row r="1094" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update- target -- dados.xlsx
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b866b217d0e5359/Área de Trabalho/Insper/2o semestre/Ciência dos Dados/Projeto 1/22-2b-cd-p1-grupo_joaoogp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Documents\GitHub\22-2b-cd-p1-grupo_joaoogp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{6AFCFE07-6B38-4DB7-9263-61A542C365A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDF7A654-B8AC-4640-A7F8-458DAE48C3E8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE16F76A-4393-42EB-8967-89DD696D2B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18115,8 +18115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A951" workbookViewId="0">
-      <selection activeCell="I954" sqref="I954"/>
+    <sheetView tabSelected="1" topLeftCell="A792" workbookViewId="0">
+      <selection activeCell="I806" sqref="I806"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34236,6 +34236,9 @@
       <c r="E805">
         <v>21</v>
       </c>
+      <c r="F805">
+        <v>0</v>
+      </c>
     </row>
     <row r="806" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A806" t="s">
@@ -34253,6 +34256,10 @@
       <c r="E806">
         <v>68</v>
       </c>
+      <c r="F806">
+        <v>1</v>
+      </c>
+      <c r="I806" s="3"/>
     </row>
     <row r="807" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A807" t="s">
@@ -34270,6 +34277,9 @@
       <c r="E807">
         <v>88</v>
       </c>
+      <c r="F807">
+        <v>2</v>
+      </c>
     </row>
     <row r="808" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A808" t="s">
@@ -34287,6 +34297,9 @@
       <c r="E808">
         <v>5</v>
       </c>
+      <c r="F808">
+        <v>1</v>
+      </c>
     </row>
     <row r="809" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A809" t="s">
@@ -34304,6 +34317,9 @@
       <c r="E809">
         <v>82</v>
       </c>
+      <c r="F809">
+        <v>2</v>
+      </c>
     </row>
     <row r="810" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A810" t="s">
@@ -34321,6 +34337,9 @@
       <c r="E810">
         <v>11</v>
       </c>
+      <c r="F810">
+        <v>1</v>
+      </c>
     </row>
     <row r="811" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A811" t="s">
@@ -34338,6 +34357,9 @@
       <c r="E811">
         <v>26</v>
       </c>
+      <c r="F811">
+        <v>2</v>
+      </c>
     </row>
     <row r="812" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A812" t="s">
@@ -34355,6 +34377,9 @@
       <c r="E812">
         <v>24</v>
       </c>
+      <c r="F812">
+        <v>1</v>
+      </c>
     </row>
     <row r="813" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A813" t="s">
@@ -34372,6 +34397,9 @@
       <c r="E813">
         <v>56</v>
       </c>
+      <c r="F813">
+        <v>1</v>
+      </c>
     </row>
     <row r="814" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A814" t="s">
@@ -34389,6 +34417,9 @@
       <c r="E814">
         <v>23</v>
       </c>
+      <c r="F814">
+        <v>1</v>
+      </c>
     </row>
     <row r="815" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A815" t="s">
@@ -34406,6 +34437,9 @@
       <c r="E815">
         <v>81</v>
       </c>
+      <c r="F815">
+        <v>1</v>
+      </c>
     </row>
     <row r="816" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A816" t="s">
@@ -34423,8 +34457,11 @@
       <c r="E816">
         <v>2</v>
       </c>
-    </row>
-    <row r="817" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F816">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="817" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A817" t="s">
         <v>6</v>
       </c>
@@ -34440,8 +34477,11 @@
       <c r="E817">
         <v>56</v>
       </c>
-    </row>
-    <row r="818" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F817">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="818" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A818" t="s">
         <v>6</v>
       </c>
@@ -34457,8 +34497,11 @@
       <c r="E818">
         <v>100</v>
       </c>
-    </row>
-    <row r="819" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F818">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="819" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A819" t="s">
         <v>6</v>
       </c>
@@ -34474,8 +34517,11 @@
       <c r="E819">
         <v>97</v>
       </c>
-    </row>
-    <row r="820" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F819">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="820" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A820" t="s">
         <v>6</v>
       </c>
@@ -34491,8 +34537,11 @@
       <c r="E820">
         <v>22</v>
       </c>
-    </row>
-    <row r="821" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F820">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="821" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A821" t="s">
         <v>6</v>
       </c>
@@ -34508,8 +34557,11 @@
       <c r="E821">
         <v>15</v>
       </c>
-    </row>
-    <row r="822" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F821">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="822" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A822" t="s">
         <v>6</v>
       </c>
@@ -34525,8 +34577,11 @@
       <c r="E822">
         <v>37</v>
       </c>
-    </row>
-    <row r="823" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F822">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="823" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A823" t="s">
         <v>6</v>
       </c>
@@ -34542,8 +34597,11 @@
       <c r="E823">
         <v>87</v>
       </c>
-    </row>
-    <row r="824" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F823">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="824" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A824" t="s">
         <v>6</v>
       </c>
@@ -34559,8 +34617,11 @@
       <c r="E824">
         <v>9</v>
       </c>
-    </row>
-    <row r="825" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F824">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="825" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A825" t="s">
         <v>6</v>
       </c>
@@ -34576,8 +34637,11 @@
       <c r="E825">
         <v>22</v>
       </c>
-    </row>
-    <row r="826" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F825">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="826" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A826" t="s">
         <v>6</v>
       </c>
@@ -34593,8 +34657,11 @@
       <c r="E826">
         <v>18</v>
       </c>
-    </row>
-    <row r="827" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F826">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="827" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A827" t="s">
         <v>6</v>
       </c>
@@ -34610,8 +34677,11 @@
       <c r="E827">
         <v>56</v>
       </c>
-    </row>
-    <row r="828" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F827">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="828" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A828" t="s">
         <v>6</v>
       </c>
@@ -34627,8 +34697,11 @@
       <c r="E828">
         <v>16</v>
       </c>
-    </row>
-    <row r="829" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F828">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="829" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A829" t="s">
         <v>6</v>
       </c>
@@ -34644,8 +34717,11 @@
       <c r="E829">
         <v>70</v>
       </c>
-    </row>
-    <row r="830" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F829">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="830" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A830" t="s">
         <v>6</v>
       </c>
@@ -34661,8 +34737,11 @@
       <c r="E830">
         <v>51</v>
       </c>
-    </row>
-    <row r="831" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F830">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="831" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A831" t="s">
         <v>6</v>
       </c>
@@ -34678,8 +34757,11 @@
       <c r="E831">
         <v>58</v>
       </c>
-    </row>
-    <row r="832" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F831">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="832" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A832" t="s">
         <v>6</v>
       </c>
@@ -34695,8 +34777,11 @@
       <c r="E832">
         <v>44</v>
       </c>
-    </row>
-    <row r="833" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F832">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="833" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A833" t="s">
         <v>6</v>
       </c>
@@ -34712,8 +34797,11 @@
       <c r="E833">
         <v>37</v>
       </c>
-    </row>
-    <row r="834" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F833">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="834" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A834" t="s">
         <v>6</v>
       </c>
@@ -34729,8 +34817,11 @@
       <c r="E834">
         <v>87</v>
       </c>
-    </row>
-    <row r="835" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F834">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="835" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A835" t="s">
         <v>6</v>
       </c>
@@ -34746,8 +34837,11 @@
       <c r="E835">
         <v>18</v>
       </c>
-    </row>
-    <row r="836" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F835">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="836" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A836" t="s">
         <v>6</v>
       </c>
@@ -34763,8 +34857,11 @@
       <c r="E836">
         <v>40</v>
       </c>
-    </row>
-    <row r="837" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F836">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="837" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A837" t="s">
         <v>6</v>
       </c>
@@ -34780,8 +34877,11 @@
       <c r="E837">
         <v>32</v>
       </c>
-    </row>
-    <row r="838" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F837">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="838" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A838" t="s">
         <v>6</v>
       </c>
@@ -34797,8 +34897,11 @@
       <c r="E838">
         <v>30</v>
       </c>
-    </row>
-    <row r="839" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F838">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="839" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A839" t="s">
         <v>6</v>
       </c>
@@ -34814,8 +34917,11 @@
       <c r="E839">
         <v>98</v>
       </c>
-    </row>
-    <row r="840" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F839">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="840" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A840" t="s">
         <v>6</v>
       </c>
@@ -34831,8 +34937,11 @@
       <c r="E840">
         <v>56</v>
       </c>
-    </row>
-    <row r="841" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F840">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="841" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A841" t="s">
         <v>6</v>
       </c>
@@ -34848,8 +34957,11 @@
       <c r="E841">
         <v>96</v>
       </c>
-    </row>
-    <row r="842" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F841">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="842" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A842" t="s">
         <v>6</v>
       </c>
@@ -34865,8 +34977,11 @@
       <c r="E842">
         <v>25</v>
       </c>
-    </row>
-    <row r="843" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F842">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="843" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A843" t="s">
         <v>6</v>
       </c>
@@ -34882,8 +34997,11 @@
       <c r="E843">
         <v>31</v>
       </c>
-    </row>
-    <row r="844" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F843">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="844" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A844" t="s">
         <v>6</v>
       </c>
@@ -34899,8 +35017,11 @@
       <c r="E844">
         <v>29</v>
       </c>
-    </row>
-    <row r="845" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F844">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="845" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A845" t="s">
         <v>6</v>
       </c>
@@ -34916,8 +35037,11 @@
       <c r="E845">
         <v>99</v>
       </c>
-    </row>
-    <row r="846" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F845">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="846" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A846" t="s">
         <v>6</v>
       </c>
@@ -34933,8 +35057,11 @@
       <c r="E846">
         <v>47</v>
       </c>
-    </row>
-    <row r="847" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F846">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="847" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A847" t="s">
         <v>6</v>
       </c>
@@ -34950,8 +35077,11 @@
       <c r="E847">
         <v>38</v>
       </c>
-    </row>
-    <row r="848" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F847">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="848" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A848" t="s">
         <v>6</v>
       </c>
@@ -34967,8 +35097,11 @@
       <c r="E848">
         <v>1</v>
       </c>
-    </row>
-    <row r="849" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F848">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="849" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A849" t="s">
         <v>6</v>
       </c>
@@ -34984,8 +35117,11 @@
       <c r="E849">
         <v>83</v>
       </c>
-    </row>
-    <row r="850" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F849">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="850" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A850" t="s">
         <v>6</v>
       </c>
@@ -35001,8 +35137,11 @@
       <c r="E850">
         <v>45</v>
       </c>
-    </row>
-    <row r="851" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F850">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="851" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A851" t="s">
         <v>6</v>
       </c>
@@ -35018,8 +35157,11 @@
       <c r="E851">
         <v>8</v>
       </c>
-    </row>
-    <row r="852" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F851">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="852" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A852" t="s">
         <v>6</v>
       </c>
@@ -35035,8 +35177,11 @@
       <c r="E852">
         <v>36</v>
       </c>
-    </row>
-    <row r="853" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F852">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="853" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A853" t="s">
         <v>6</v>
       </c>
@@ -35052,8 +35197,11 @@
       <c r="E853">
         <v>82</v>
       </c>
-    </row>
-    <row r="854" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F853">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="854" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A854" t="s">
         <v>6</v>
       </c>
@@ -35069,8 +35217,11 @@
       <c r="E854">
         <v>8</v>
       </c>
-    </row>
-    <row r="855" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F854">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="855" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A855" t="s">
         <v>6</v>
       </c>
@@ -35086,8 +35237,11 @@
       <c r="E855">
         <v>7</v>
       </c>
-    </row>
-    <row r="856" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F855">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="856" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A856" t="s">
         <v>6</v>
       </c>
@@ -35103,8 +35257,11 @@
       <c r="E856">
         <v>36</v>
       </c>
-    </row>
-    <row r="857" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F856">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="857" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A857" t="s">
         <v>6</v>
       </c>
@@ -35120,8 +35277,11 @@
       <c r="E857">
         <v>76</v>
       </c>
-    </row>
-    <row r="858" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F857">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="858" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A858" t="s">
         <v>6</v>
       </c>
@@ -35137,8 +35297,11 @@
       <c r="E858">
         <v>27</v>
       </c>
-    </row>
-    <row r="859" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F858">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="859" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A859" t="s">
         <v>6</v>
       </c>
@@ -35154,8 +35317,11 @@
       <c r="E859">
         <v>91</v>
       </c>
-    </row>
-    <row r="860" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F859">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="860" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A860" t="s">
         <v>6</v>
       </c>
@@ -35171,8 +35337,11 @@
       <c r="E860">
         <v>45</v>
       </c>
-    </row>
-    <row r="861" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F860">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="861" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A861" t="s">
         <v>6</v>
       </c>
@@ -35188,8 +35357,11 @@
       <c r="E861">
         <v>11</v>
       </c>
-    </row>
-    <row r="862" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F861">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="862" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A862" t="s">
         <v>6</v>
       </c>
@@ -35205,8 +35377,11 @@
       <c r="E862">
         <v>43</v>
       </c>
-    </row>
-    <row r="863" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F862">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="863" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A863" t="s">
         <v>6</v>
       </c>
@@ -35222,8 +35397,11 @@
       <c r="E863">
         <v>1</v>
       </c>
-    </row>
-    <row r="864" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F863">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="864" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A864" t="s">
         <v>6</v>
       </c>
@@ -35239,8 +35417,11 @@
       <c r="E864">
         <v>92</v>
       </c>
-    </row>
-    <row r="865" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F864">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="865" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A865" t="s">
         <v>6</v>
       </c>
@@ -35256,8 +35437,11 @@
       <c r="E865">
         <v>39</v>
       </c>
-    </row>
-    <row r="866" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F865">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="866" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A866" t="s">
         <v>6</v>
       </c>
@@ -35273,8 +35457,11 @@
       <c r="E866">
         <v>59</v>
       </c>
-    </row>
-    <row r="867" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F866">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="867" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A867" t="s">
         <v>6</v>
       </c>
@@ -35290,8 +35477,11 @@
       <c r="E867">
         <v>40</v>
       </c>
-    </row>
-    <row r="868" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F867">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="868" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A868" t="s">
         <v>6</v>
       </c>
@@ -35307,8 +35497,11 @@
       <c r="E868">
         <v>86</v>
       </c>
-    </row>
-    <row r="869" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F868">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="869" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A869" t="s">
         <v>6</v>
       </c>
@@ -35324,8 +35517,11 @@
       <c r="E869">
         <v>52</v>
       </c>
-    </row>
-    <row r="870" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F869">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="870" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A870" t="s">
         <v>6</v>
       </c>
@@ -35341,8 +35537,11 @@
       <c r="E870">
         <v>69</v>
       </c>
-    </row>
-    <row r="871" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F870">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="871" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A871" t="s">
         <v>6</v>
       </c>
@@ -35358,8 +35557,11 @@
       <c r="E871">
         <v>69</v>
       </c>
-    </row>
-    <row r="872" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F871">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="872" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A872" t="s">
         <v>6</v>
       </c>
@@ -35375,8 +35577,11 @@
       <c r="E872">
         <v>91</v>
       </c>
-    </row>
-    <row r="873" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F872">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="873" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A873" t="s">
         <v>6</v>
       </c>
@@ -35392,8 +35597,11 @@
       <c r="E873">
         <v>52</v>
       </c>
-    </row>
-    <row r="874" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F873">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="874" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A874" t="s">
         <v>6</v>
       </c>
@@ -35409,8 +35617,11 @@
       <c r="E874">
         <v>76</v>
       </c>
-    </row>
-    <row r="875" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F874">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="875" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A875" t="s">
         <v>6</v>
       </c>
@@ -35426,8 +35637,11 @@
       <c r="E875">
         <v>97</v>
       </c>
-    </row>
-    <row r="876" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F875">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="876" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A876" t="s">
         <v>6</v>
       </c>
@@ -35443,8 +35657,11 @@
       <c r="E876">
         <v>94</v>
       </c>
-    </row>
-    <row r="877" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F876">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="877" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A877" t="s">
         <v>6</v>
       </c>
@@ -35460,8 +35677,11 @@
       <c r="E877">
         <v>70</v>
       </c>
-    </row>
-    <row r="878" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F877">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="878" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A878" t="s">
         <v>6</v>
       </c>
@@ -35477,8 +35697,11 @@
       <c r="E878">
         <v>2</v>
       </c>
-    </row>
-    <row r="879" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F878">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="879" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A879" t="s">
         <v>6</v>
       </c>
@@ -35494,8 +35717,11 @@
       <c r="E879">
         <v>57</v>
       </c>
-    </row>
-    <row r="880" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F879">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="880" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A880" t="s">
         <v>6</v>
       </c>
@@ -35511,8 +35737,11 @@
       <c r="E880">
         <v>51</v>
       </c>
-    </row>
-    <row r="881" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F880">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="881" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A881" t="s">
         <v>6</v>
       </c>
@@ -35528,8 +35757,11 @@
       <c r="E881">
         <v>56</v>
       </c>
-    </row>
-    <row r="882" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F881">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="882" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A882" t="s">
         <v>6</v>
       </c>
@@ -35545,8 +35777,11 @@
       <c r="E882">
         <v>54</v>
       </c>
-    </row>
-    <row r="883" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F882">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="883" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A883" t="s">
         <v>6</v>
       </c>
@@ -35562,8 +35797,11 @@
       <c r="E883">
         <v>22</v>
       </c>
-    </row>
-    <row r="884" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F883">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="884" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A884" t="s">
         <v>6</v>
       </c>
@@ -35579,8 +35817,11 @@
       <c r="E884">
         <v>19</v>
       </c>
-    </row>
-    <row r="885" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F884">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="885" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A885" t="s">
         <v>6</v>
       </c>
@@ -35596,8 +35837,11 @@
       <c r="E885">
         <v>95</v>
       </c>
-    </row>
-    <row r="886" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F885">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="886" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A886" t="s">
         <v>6</v>
       </c>
@@ -35613,8 +35857,11 @@
       <c r="E886">
         <v>64</v>
       </c>
-    </row>
-    <row r="887" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F886">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="887" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A887" t="s">
         <v>6</v>
       </c>
@@ -35630,8 +35877,11 @@
       <c r="E887">
         <v>49</v>
       </c>
-    </row>
-    <row r="888" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F887">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="888" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A888" t="s">
         <v>6</v>
       </c>
@@ -35647,8 +35897,11 @@
       <c r="E888">
         <v>62</v>
       </c>
-    </row>
-    <row r="889" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F888">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="889" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A889" t="s">
         <v>6</v>
       </c>
@@ -35664,8 +35917,11 @@
       <c r="E889">
         <v>73</v>
       </c>
-    </row>
-    <row r="890" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F889">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="890" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A890" t="s">
         <v>6</v>
       </c>
@@ -35681,8 +35937,11 @@
       <c r="E890">
         <v>24</v>
       </c>
-    </row>
-    <row r="891" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F890">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="891" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A891" t="s">
         <v>6</v>
       </c>
@@ -35698,8 +35957,11 @@
       <c r="E891">
         <v>13</v>
       </c>
-    </row>
-    <row r="892" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F891">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="892" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A892" t="s">
         <v>6</v>
       </c>
@@ -35715,8 +35977,11 @@
       <c r="E892">
         <v>72</v>
       </c>
-    </row>
-    <row r="893" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F892">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="893" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A893" t="s">
         <v>6</v>
       </c>
@@ -35732,8 +35997,11 @@
       <c r="E893">
         <v>72</v>
       </c>
-    </row>
-    <row r="894" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F893">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="894" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A894" t="s">
         <v>6</v>
       </c>
@@ -35749,8 +36017,11 @@
       <c r="E894">
         <v>53</v>
       </c>
-    </row>
-    <row r="895" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F894">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="895" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A895" t="s">
         <v>6</v>
       </c>
@@ -35766,8 +36037,11 @@
       <c r="E895">
         <v>68</v>
       </c>
-    </row>
-    <row r="896" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F895">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="896" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A896" t="s">
         <v>6</v>
       </c>
@@ -35783,8 +36057,11 @@
       <c r="E896">
         <v>24</v>
       </c>
-    </row>
-    <row r="897" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F896">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="897" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A897" t="s">
         <v>6</v>
       </c>
@@ -35800,8 +36077,11 @@
       <c r="E897">
         <v>31</v>
       </c>
-    </row>
-    <row r="898" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F897">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="898" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A898" t="s">
         <v>6</v>
       </c>
@@ -35817,8 +36097,11 @@
       <c r="E898">
         <v>49</v>
       </c>
-    </row>
-    <row r="899" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F898">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="899" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A899" t="s">
         <v>6</v>
       </c>
@@ -35834,8 +36117,11 @@
       <c r="E899">
         <v>65</v>
       </c>
-    </row>
-    <row r="900" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F899">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="900" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A900" t="s">
         <v>6</v>
       </c>
@@ -35851,8 +36137,11 @@
       <c r="E900">
         <v>90</v>
       </c>
-    </row>
-    <row r="901" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F900">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="901" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A901" t="s">
         <v>6</v>
       </c>
@@ -35868,8 +36157,11 @@
       <c r="E901">
         <v>21</v>
       </c>
-    </row>
-    <row r="902" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F901">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="902" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A902" t="s">
         <v>6</v>
       </c>
@@ -35885,8 +36177,11 @@
       <c r="E902">
         <v>82</v>
       </c>
-    </row>
-    <row r="903" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F902">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="903" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A903" t="s">
         <v>6</v>
       </c>
@@ -35902,8 +36197,11 @@
       <c r="E903">
         <v>46</v>
       </c>
-    </row>
-    <row r="904" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F903">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="904" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A904" t="s">
         <v>6</v>
       </c>
@@ -35919,8 +36217,11 @@
       <c r="E904">
         <v>32</v>
       </c>
-    </row>
-    <row r="905" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F904">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="905" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A905" t="s">
         <v>6</v>
       </c>
@@ -35936,8 +36237,11 @@
       <c r="E905">
         <v>32</v>
       </c>
-    </row>
-    <row r="906" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F905">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="906" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A906" t="s">
         <v>6</v>
       </c>
@@ -35953,8 +36257,11 @@
       <c r="E906">
         <v>68</v>
       </c>
-    </row>
-    <row r="907" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F906">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="907" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A907" t="s">
         <v>6</v>
       </c>
@@ -35970,8 +36277,11 @@
       <c r="E907">
         <v>27</v>
       </c>
-    </row>
-    <row r="908" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F907">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="908" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A908" t="s">
         <v>6</v>
       </c>
@@ -35987,8 +36297,11 @@
       <c r="E908">
         <v>68</v>
       </c>
-    </row>
-    <row r="909" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F908">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="909" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A909" t="s">
         <v>6</v>
       </c>
@@ -36004,8 +36317,11 @@
       <c r="E909">
         <v>17</v>
       </c>
-    </row>
-    <row r="910" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F909">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="910" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A910" t="s">
         <v>6</v>
       </c>
@@ -36021,8 +36337,11 @@
       <c r="E910">
         <v>68</v>
       </c>
-    </row>
-    <row r="911" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F910">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="911" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A911" t="s">
         <v>6</v>
       </c>
@@ -36038,8 +36357,11 @@
       <c r="E911">
         <v>52</v>
       </c>
-    </row>
-    <row r="912" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F911">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="912" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A912" t="s">
         <v>6</v>
       </c>
@@ -36055,8 +36377,11 @@
       <c r="E912">
         <v>86</v>
       </c>
-    </row>
-    <row r="913" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F912">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="913" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A913" t="s">
         <v>6</v>
       </c>
@@ -36072,8 +36397,11 @@
       <c r="E913">
         <v>29</v>
       </c>
-    </row>
-    <row r="914" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F913">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="914" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A914" t="s">
         <v>6</v>
       </c>
@@ -36089,8 +36417,11 @@
       <c r="E914">
         <v>73</v>
       </c>
-    </row>
-    <row r="915" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F914">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="915" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A915" t="s">
         <v>6</v>
       </c>
@@ -36106,8 +36437,11 @@
       <c r="E915">
         <v>23</v>
       </c>
-    </row>
-    <row r="916" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F915">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="916" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A916" t="s">
         <v>6</v>
       </c>
@@ -36123,8 +36457,11 @@
       <c r="E916">
         <v>18</v>
       </c>
-    </row>
-    <row r="917" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F916">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="917" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A917" t="s">
         <v>6</v>
       </c>
@@ -36140,8 +36477,11 @@
       <c r="E917">
         <v>97</v>
       </c>
-    </row>
-    <row r="918" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F917">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="918" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A918" t="s">
         <v>6</v>
       </c>
@@ -36157,8 +36497,11 @@
       <c r="E918">
         <v>74</v>
       </c>
-    </row>
-    <row r="919" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F918">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="919" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A919" t="s">
         <v>6</v>
       </c>
@@ -36174,8 +36517,11 @@
       <c r="E919">
         <v>16</v>
       </c>
-    </row>
-    <row r="920" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F919">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="920" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A920" t="s">
         <v>6</v>
       </c>
@@ -36191,8 +36537,11 @@
       <c r="E920">
         <v>100</v>
       </c>
-    </row>
-    <row r="921" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F920">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="921" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A921" t="s">
         <v>6</v>
       </c>
@@ -36208,8 +36557,11 @@
       <c r="E921">
         <v>36</v>
       </c>
-    </row>
-    <row r="922" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F921">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="922" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A922" t="s">
         <v>6</v>
       </c>
@@ -36225,8 +36577,11 @@
       <c r="E922">
         <v>56</v>
       </c>
-    </row>
-    <row r="923" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F922">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="923" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A923" t="s">
         <v>6</v>
       </c>
@@ -36242,8 +36597,11 @@
       <c r="E923">
         <v>8</v>
       </c>
-    </row>
-    <row r="924" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F923">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="924" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A924" t="s">
         <v>6</v>
       </c>
@@ -36259,8 +36617,11 @@
       <c r="E924">
         <v>67</v>
       </c>
-    </row>
-    <row r="925" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F924">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="925" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A925" t="s">
         <v>6</v>
       </c>
@@ -36276,8 +36637,11 @@
       <c r="E925">
         <v>86</v>
       </c>
-    </row>
-    <row r="926" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F925">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="926" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A926" t="s">
         <v>6</v>
       </c>
@@ -36293,8 +36657,11 @@
       <c r="E926">
         <v>11</v>
       </c>
-    </row>
-    <row r="927" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F926">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="927" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A927" t="s">
         <v>6</v>
       </c>
@@ -36310,8 +36677,11 @@
       <c r="E927">
         <v>6</v>
       </c>
-    </row>
-    <row r="928" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F927">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="928" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A928" t="s">
         <v>6</v>
       </c>
@@ -36327,8 +36697,11 @@
       <c r="E928">
         <v>37</v>
       </c>
-    </row>
-    <row r="929" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F928">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="929" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A929" t="s">
         <v>6</v>
       </c>
@@ -36344,8 +36717,11 @@
       <c r="E929">
         <v>51</v>
       </c>
-    </row>
-    <row r="930" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F929">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="930" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A930" t="s">
         <v>6</v>
       </c>
@@ -36361,8 +36737,11 @@
       <c r="E930">
         <v>96</v>
       </c>
-    </row>
-    <row r="931" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F930">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="931" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A931" t="s">
         <v>6</v>
       </c>
@@ -36378,8 +36757,11 @@
       <c r="E931">
         <v>53</v>
       </c>
-    </row>
-    <row r="932" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F931">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="932" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A932" t="s">
         <v>6</v>
       </c>
@@ -36395,8 +36777,11 @@
       <c r="E932">
         <v>91</v>
       </c>
-    </row>
-    <row r="933" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F932">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="933" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A933" t="s">
         <v>6</v>
       </c>
@@ -36412,8 +36797,11 @@
       <c r="E933">
         <v>87</v>
       </c>
-    </row>
-    <row r="934" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F933">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="934" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A934" t="s">
         <v>6</v>
       </c>
@@ -36429,8 +36817,11 @@
       <c r="E934">
         <v>29</v>
       </c>
-    </row>
-    <row r="935" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F934">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="935" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A935" t="s">
         <v>6</v>
       </c>
@@ -36446,8 +36837,11 @@
       <c r="E935">
         <v>25</v>
       </c>
-    </row>
-    <row r="936" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F935">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="936" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A936" t="s">
         <v>6</v>
       </c>
@@ -36463,8 +36857,11 @@
       <c r="E936">
         <v>36</v>
       </c>
-    </row>
-    <row r="937" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F936">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="937" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A937" t="s">
         <v>6</v>
       </c>
@@ -36480,8 +36877,11 @@
       <c r="E937">
         <v>88</v>
       </c>
-    </row>
-    <row r="938" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F937">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="938" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A938" t="s">
         <v>6</v>
       </c>
@@ -36497,8 +36897,11 @@
       <c r="E938">
         <v>41</v>
       </c>
-    </row>
-    <row r="939" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F938">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="939" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A939" t="s">
         <v>6</v>
       </c>
@@ -36514,8 +36917,11 @@
       <c r="E939">
         <v>80</v>
       </c>
-    </row>
-    <row r="940" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F939">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="940" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A940" t="s">
         <v>6</v>
       </c>
@@ -36531,8 +36937,11 @@
       <c r="E940">
         <v>52</v>
       </c>
-    </row>
-    <row r="941" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F940">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="941" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A941" t="s">
         <v>6</v>
       </c>
@@ -36548,8 +36957,11 @@
       <c r="E941">
         <v>34</v>
       </c>
-    </row>
-    <row r="942" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F941">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="942" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A942" t="s">
         <v>6</v>
       </c>
@@ -36565,8 +36977,11 @@
       <c r="E942">
         <v>93</v>
       </c>
-    </row>
-    <row r="943" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F942">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="943" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A943" t="s">
         <v>6</v>
       </c>
@@ -36582,8 +36997,11 @@
       <c r="E943">
         <v>28</v>
       </c>
-    </row>
-    <row r="944" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F943">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="944" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A944" t="s">
         <v>6</v>
       </c>
@@ -36599,6 +37017,9 @@
       <c r="E944">
         <v>35</v>
       </c>
+      <c r="F944">
+        <v>1</v>
+      </c>
     </row>
     <row r="945" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A945" t="s">
@@ -36616,6 +37037,9 @@
       <c r="E945">
         <v>6</v>
       </c>
+      <c r="F945">
+        <v>1</v>
+      </c>
     </row>
     <row r="946" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A946" t="s">
@@ -36633,6 +37057,9 @@
       <c r="E946">
         <v>66</v>
       </c>
+      <c r="F946">
+        <v>1</v>
+      </c>
     </row>
     <row r="947" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A947" t="s">
@@ -36650,6 +37077,9 @@
       <c r="E947">
         <v>95</v>
       </c>
+      <c r="F947">
+        <v>1</v>
+      </c>
     </row>
     <row r="948" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A948" t="s">
@@ -36667,6 +37097,9 @@
       <c r="E948">
         <v>1</v>
       </c>
+      <c r="F948">
+        <v>1</v>
+      </c>
     </row>
     <row r="949" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A949" t="s">
@@ -36684,6 +37117,9 @@
       <c r="E949">
         <v>9</v>
       </c>
+      <c r="F949">
+        <v>2</v>
+      </c>
     </row>
     <row r="950" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A950" t="s">
@@ -36700,6 +37136,9 @@
       </c>
       <c r="E950">
         <v>47</v>
+      </c>
+      <c r="F950">
+        <v>0</v>
       </c>
     </row>
     <row r="951" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update-planilha teste no banco de dados
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b866b217d0e5359/Área de Trabalho/Insper/2o semestre/Ciência dos Dados/Projeto 1/22-2b-cd-p1-grupo_joaoogp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Documents\GitHub\22-2b-cd-p1-grupo_joaoogp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{503ED185-6242-4B49-B639-BC64EE51E67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2DED24F-DA19-417E-B907-D6D976790D8C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72378759-B21A-47BB-A5C8-3482E4BBCCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8015" uniqueCount="5893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8016" uniqueCount="5894">
   <si>
     <t>Categoria</t>
   </si>
@@ -17700,6 +17700,9 @@
   </si>
   <si>
     <t>neutra</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
 </sst>
 </file>
@@ -42171,8 +42174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H801"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A796" workbookViewId="0">
-      <selection activeCell="F625" sqref="F625:F801"/>
+    <sheetView tabSelected="1" topLeftCell="A572" workbookViewId="0">
+      <selection activeCell="F582" sqref="F582"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50178,7 +50181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>6</v>
       </c>
@@ -50194,8 +50197,11 @@
       <c r="E401">
         <v>25</v>
       </c>
-    </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F401">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>6</v>
       </c>
@@ -50211,8 +50217,14 @@
       <c r="E402">
         <v>7</v>
       </c>
-    </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F402">
+        <v>1</v>
+      </c>
+      <c r="G402" t="s">
+        <v>5893</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>6</v>
       </c>
@@ -50228,8 +50240,11 @@
       <c r="E403">
         <v>33</v>
       </c>
-    </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F403">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>6</v>
       </c>
@@ -50245,8 +50260,11 @@
       <c r="E404">
         <v>36</v>
       </c>
-    </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F404">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>6</v>
       </c>
@@ -50262,8 +50280,11 @@
       <c r="E405">
         <v>50</v>
       </c>
-    </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F405">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>6</v>
       </c>
@@ -50279,8 +50300,11 @@
       <c r="E406">
         <v>18</v>
       </c>
-    </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F406">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>6</v>
       </c>
@@ -50296,8 +50320,11 @@
       <c r="E407">
         <v>5</v>
       </c>
-    </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>6</v>
       </c>
@@ -50313,8 +50340,11 @@
       <c r="E408">
         <v>18</v>
       </c>
-    </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F408">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>6</v>
       </c>
@@ -50330,8 +50360,11 @@
       <c r="E409">
         <v>28</v>
       </c>
-    </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F409">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>6</v>
       </c>
@@ -50347,8 +50380,11 @@
       <c r="E410">
         <v>51</v>
       </c>
-    </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F410">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>6</v>
       </c>
@@ -50364,8 +50400,11 @@
       <c r="E411">
         <v>15</v>
       </c>
-    </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F411">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>6</v>
       </c>
@@ -50381,8 +50420,11 @@
       <c r="E412">
         <v>84</v>
       </c>
-    </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>6</v>
       </c>
@@ -50398,8 +50440,11 @@
       <c r="E413">
         <v>71</v>
       </c>
-    </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>6</v>
       </c>
@@ -50415,8 +50460,11 @@
       <c r="E414">
         <v>56</v>
       </c>
-    </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F414">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>6</v>
       </c>
@@ -50432,8 +50480,11 @@
       <c r="E415">
         <v>34</v>
       </c>
-    </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F415">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>6</v>
       </c>
@@ -50449,8 +50500,11 @@
       <c r="E416">
         <v>98</v>
       </c>
-    </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F416">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>6</v>
       </c>
@@ -50466,8 +50520,11 @@
       <c r="E417">
         <v>95</v>
       </c>
-    </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>6</v>
       </c>
@@ -50483,8 +50540,11 @@
       <c r="E418">
         <v>98</v>
       </c>
-    </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F418">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>6</v>
       </c>
@@ -50500,8 +50560,11 @@
       <c r="E419">
         <v>30</v>
       </c>
-    </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F419">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>6</v>
       </c>
@@ -50517,8 +50580,11 @@
       <c r="E420">
         <v>62</v>
       </c>
-    </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F420">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>6</v>
       </c>
@@ -50534,8 +50600,11 @@
       <c r="E421">
         <v>27</v>
       </c>
-    </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F421">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>6</v>
       </c>
@@ -50551,8 +50620,11 @@
       <c r="E422">
         <v>43</v>
       </c>
-    </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F422">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>6</v>
       </c>
@@ -50568,8 +50640,11 @@
       <c r="E423">
         <v>75</v>
       </c>
-    </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F423">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>6</v>
       </c>
@@ -50585,8 +50660,11 @@
       <c r="E424">
         <v>58</v>
       </c>
-    </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F424">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>6</v>
       </c>
@@ -50602,8 +50680,11 @@
       <c r="E425">
         <v>81</v>
       </c>
-    </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F425">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>6</v>
       </c>
@@ -50619,8 +50700,11 @@
       <c r="E426">
         <v>60</v>
       </c>
-    </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>6</v>
       </c>
@@ -50636,8 +50720,11 @@
       <c r="E427">
         <v>35</v>
       </c>
-    </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F427">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>6</v>
       </c>
@@ -50653,8 +50740,11 @@
       <c r="E428">
         <v>80</v>
       </c>
-    </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F428">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>6</v>
       </c>
@@ -50670,8 +50760,11 @@
       <c r="E429">
         <v>26</v>
       </c>
-    </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F429">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>6</v>
       </c>
@@ -50687,8 +50780,11 @@
       <c r="E430">
         <v>32</v>
       </c>
-    </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F430">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>6</v>
       </c>
@@ -50704,8 +50800,11 @@
       <c r="E431">
         <v>82</v>
       </c>
-    </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F431">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>6</v>
       </c>
@@ -50721,8 +50820,11 @@
       <c r="E432">
         <v>18</v>
       </c>
-    </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F432">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>6</v>
       </c>
@@ -50738,8 +50840,11 @@
       <c r="E433">
         <v>29</v>
       </c>
-    </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>6</v>
       </c>
@@ -50755,8 +50860,11 @@
       <c r="E434">
         <v>95</v>
       </c>
-    </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F434">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>6</v>
       </c>
@@ -50772,8 +50880,11 @@
       <c r="E435">
         <v>3</v>
       </c>
-    </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F435">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>6</v>
       </c>
@@ -50789,8 +50900,11 @@
       <c r="E436">
         <v>25</v>
       </c>
-    </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F436">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>6</v>
       </c>
@@ -50806,8 +50920,11 @@
       <c r="E437">
         <v>12</v>
       </c>
-    </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>6</v>
       </c>
@@ -50823,8 +50940,11 @@
       <c r="E438">
         <v>12</v>
       </c>
-    </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>6</v>
       </c>
@@ -50840,8 +50960,11 @@
       <c r="E439">
         <v>90</v>
       </c>
-    </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F439">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>6</v>
       </c>
@@ -50857,8 +50980,11 @@
       <c r="E440">
         <v>52</v>
       </c>
-    </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F440">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>6</v>
       </c>
@@ -50874,8 +51000,11 @@
       <c r="E441">
         <v>55</v>
       </c>
-    </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F441">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>6</v>
       </c>
@@ -50891,8 +51020,11 @@
       <c r="E442">
         <v>80</v>
       </c>
-    </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F442">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>6</v>
       </c>
@@ -50908,8 +51040,11 @@
       <c r="E443">
         <v>60</v>
       </c>
-    </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F443">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>6</v>
       </c>
@@ -50925,8 +51060,11 @@
       <c r="E444">
         <v>74</v>
       </c>
-    </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F444">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>6</v>
       </c>
@@ -50942,8 +51080,11 @@
       <c r="E445">
         <v>72</v>
       </c>
-    </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F445">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>6</v>
       </c>
@@ -50959,8 +51100,11 @@
       <c r="E446">
         <v>7</v>
       </c>
-    </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>6</v>
       </c>
@@ -50976,8 +51120,11 @@
       <c r="E447">
         <v>61</v>
       </c>
-    </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F447">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
         <v>6</v>
       </c>
@@ -50993,8 +51140,11 @@
       <c r="E448">
         <v>17</v>
       </c>
-    </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F448">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>6</v>
       </c>
@@ -51010,8 +51160,11 @@
       <c r="E449">
         <v>41</v>
       </c>
-    </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F449">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
         <v>6</v>
       </c>
@@ -51027,8 +51180,11 @@
       <c r="E450">
         <v>78</v>
       </c>
-    </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F450">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>6</v>
       </c>
@@ -51044,8 +51200,11 @@
       <c r="E451">
         <v>30</v>
       </c>
-    </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F451">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
         <v>6</v>
       </c>
@@ -51061,8 +51220,11 @@
       <c r="E452">
         <v>79</v>
       </c>
-    </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F452">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>6</v>
       </c>
@@ -51078,8 +51240,11 @@
       <c r="E453">
         <v>23</v>
       </c>
-    </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F453">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>6</v>
       </c>
@@ -51095,8 +51260,11 @@
       <c r="E454">
         <v>100</v>
       </c>
-    </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F454">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>6</v>
       </c>
@@ -51112,8 +51280,11 @@
       <c r="E455">
         <v>26</v>
       </c>
-    </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F455">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>6</v>
       </c>
@@ -51129,8 +51300,11 @@
       <c r="E456">
         <v>26</v>
       </c>
-    </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
         <v>6</v>
       </c>
@@ -51146,8 +51320,11 @@
       <c r="E457">
         <v>79</v>
       </c>
-    </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F457">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
         <v>6</v>
       </c>
@@ -51163,8 +51340,11 @@
       <c r="E458">
         <v>62</v>
       </c>
-    </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F458">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>6</v>
       </c>
@@ -51180,8 +51360,11 @@
       <c r="E459">
         <v>23</v>
       </c>
-    </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>6</v>
       </c>
@@ -51197,8 +51380,11 @@
       <c r="E460">
         <v>78</v>
       </c>
-    </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F460">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>6</v>
       </c>
@@ -51214,8 +51400,11 @@
       <c r="E461">
         <v>83</v>
       </c>
-    </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F461">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
         <v>6</v>
       </c>
@@ -51231,8 +51420,11 @@
       <c r="E462">
         <v>48</v>
       </c>
-    </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F462">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>6</v>
       </c>
@@ -51248,8 +51440,11 @@
       <c r="E463">
         <v>20</v>
       </c>
-    </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F463">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>6</v>
       </c>
@@ -51265,8 +51460,11 @@
       <c r="E464">
         <v>25</v>
       </c>
-    </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>6</v>
       </c>
@@ -51282,8 +51480,11 @@
       <c r="E465">
         <v>29</v>
       </c>
-    </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F465">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>6</v>
       </c>
@@ -51299,8 +51500,11 @@
       <c r="E466">
         <v>76</v>
       </c>
-    </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>6</v>
       </c>
@@ -51316,8 +51520,11 @@
       <c r="E467">
         <v>58</v>
       </c>
-    </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F467">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
         <v>6</v>
       </c>
@@ -51333,8 +51540,11 @@
       <c r="E468">
         <v>42</v>
       </c>
-    </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F468">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>6</v>
       </c>
@@ -51350,8 +51560,11 @@
       <c r="E469">
         <v>88</v>
       </c>
-    </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F469">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
         <v>6</v>
       </c>
@@ -51367,8 +51580,11 @@
       <c r="E470">
         <v>79</v>
       </c>
-    </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F470">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
         <v>6</v>
       </c>
@@ -51384,8 +51600,11 @@
       <c r="E471">
         <v>21</v>
       </c>
-    </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>6</v>
       </c>
@@ -51401,8 +51620,11 @@
       <c r="E472">
         <v>42</v>
       </c>
-    </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F472">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>6</v>
       </c>
@@ -51418,8 +51640,11 @@
       <c r="E473">
         <v>80</v>
       </c>
-    </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F473">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
         <v>6</v>
       </c>
@@ -51435,8 +51660,11 @@
       <c r="E474">
         <v>47</v>
       </c>
-    </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F474">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
         <v>6</v>
       </c>
@@ -51452,8 +51680,11 @@
       <c r="E475">
         <v>74</v>
       </c>
-    </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>6</v>
       </c>
@@ -51469,8 +51700,11 @@
       <c r="E476">
         <v>97</v>
       </c>
-    </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F476">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>6</v>
       </c>
@@ -51486,8 +51720,11 @@
       <c r="E477">
         <v>16</v>
       </c>
-    </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F477">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>6</v>
       </c>
@@ -51503,8 +51740,11 @@
       <c r="E478">
         <v>28</v>
       </c>
-    </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F478">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="479" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>6</v>
       </c>
@@ -51520,8 +51760,11 @@
       <c r="E479">
         <v>91</v>
       </c>
-    </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F479">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>6</v>
       </c>
@@ -51537,8 +51780,11 @@
       <c r="E480">
         <v>6</v>
       </c>
-    </row>
-    <row r="481" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F480">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>6</v>
       </c>
@@ -51554,8 +51800,11 @@
       <c r="E481">
         <v>15</v>
       </c>
-    </row>
-    <row r="482" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F481">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>6</v>
       </c>
@@ -51571,8 +51820,11 @@
       <c r="E482">
         <v>68</v>
       </c>
-    </row>
-    <row r="483" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F482">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>6</v>
       </c>
@@ -51588,8 +51840,11 @@
       <c r="E483">
         <v>52</v>
       </c>
-    </row>
-    <row r="484" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F483">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>6</v>
       </c>
@@ -51605,8 +51860,11 @@
       <c r="E484">
         <v>41</v>
       </c>
-    </row>
-    <row r="485" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F484">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>6</v>
       </c>
@@ -51622,8 +51880,11 @@
       <c r="E485">
         <v>83</v>
       </c>
-    </row>
-    <row r="486" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F485">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
         <v>6</v>
       </c>
@@ -51639,8 +51900,11 @@
       <c r="E486">
         <v>12</v>
       </c>
-    </row>
-    <row r="487" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F486">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>6</v>
       </c>
@@ -51656,8 +51920,11 @@
       <c r="E487">
         <v>32</v>
       </c>
-    </row>
-    <row r="488" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F487">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
         <v>6</v>
       </c>
@@ -51673,8 +51940,11 @@
       <c r="E488">
         <v>10</v>
       </c>
-    </row>
-    <row r="489" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F488">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
         <v>6</v>
       </c>
@@ -51690,8 +51960,11 @@
       <c r="E489">
         <v>96</v>
       </c>
-    </row>
-    <row r="490" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F489">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
         <v>6</v>
       </c>
@@ -51707,8 +51980,11 @@
       <c r="E490">
         <v>91</v>
       </c>
-    </row>
-    <row r="491" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F490">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="491" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>6</v>
       </c>
@@ -51724,8 +52000,11 @@
       <c r="E491">
         <v>21</v>
       </c>
-    </row>
-    <row r="492" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F491">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="492" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>6</v>
       </c>
@@ -51741,8 +52020,11 @@
       <c r="E492">
         <v>73</v>
       </c>
-    </row>
-    <row r="493" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F492">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="493" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>6</v>
       </c>
@@ -51758,8 +52040,11 @@
       <c r="E493">
         <v>44</v>
       </c>
-    </row>
-    <row r="494" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F493">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>6</v>
       </c>
@@ -51775,8 +52060,11 @@
       <c r="E494">
         <v>3</v>
       </c>
-    </row>
-    <row r="495" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F494">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>6</v>
       </c>
@@ -51792,8 +52080,11 @@
       <c r="E495">
         <v>73</v>
       </c>
-    </row>
-    <row r="496" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F495">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>6</v>
       </c>
@@ -51809,8 +52100,11 @@
       <c r="E496">
         <v>94</v>
       </c>
-    </row>
-    <row r="497" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F496">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>6</v>
       </c>
@@ -51826,8 +52120,11 @@
       <c r="E497">
         <v>10</v>
       </c>
-    </row>
-    <row r="498" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F497">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>6</v>
       </c>
@@ -51843,8 +52140,11 @@
       <c r="E498">
         <v>64</v>
       </c>
-    </row>
-    <row r="499" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F498">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>6</v>
       </c>
@@ -51860,8 +52160,11 @@
       <c r="E499">
         <v>93</v>
       </c>
-    </row>
-    <row r="500" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F499">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>6</v>
       </c>
@@ -51877,8 +52180,11 @@
       <c r="E500">
         <v>68</v>
       </c>
-    </row>
-    <row r="501" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F500">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>6</v>
       </c>
@@ -51894,8 +52200,11 @@
       <c r="E501">
         <v>94</v>
       </c>
-    </row>
-    <row r="502" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F501">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>6</v>
       </c>
@@ -51911,8 +52220,11 @@
       <c r="E502">
         <v>1</v>
       </c>
-    </row>
-    <row r="503" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F502">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>6</v>
       </c>
@@ -51928,8 +52240,11 @@
       <c r="E503">
         <v>97</v>
       </c>
-    </row>
-    <row r="504" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F503">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>6</v>
       </c>
@@ -51945,8 +52260,11 @@
       <c r="E504">
         <v>22</v>
       </c>
-    </row>
-    <row r="505" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F504">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>6</v>
       </c>
@@ -51962,8 +52280,11 @@
       <c r="E505">
         <v>10</v>
       </c>
-    </row>
-    <row r="506" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F505">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>6</v>
       </c>
@@ -51979,8 +52300,11 @@
       <c r="E506">
         <v>99</v>
       </c>
-    </row>
-    <row r="507" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F506">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>6</v>
       </c>
@@ -51996,8 +52320,11 @@
       <c r="E507">
         <v>55</v>
       </c>
-    </row>
-    <row r="508" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F507">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>6</v>
       </c>
@@ -52013,8 +52340,11 @@
       <c r="E508">
         <v>2</v>
       </c>
-    </row>
-    <row r="509" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F508">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>6</v>
       </c>
@@ -52030,8 +52360,11 @@
       <c r="E509">
         <v>72</v>
       </c>
-    </row>
-    <row r="510" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F509">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>6</v>
       </c>
@@ -52047,8 +52380,11 @@
       <c r="E510">
         <v>80</v>
       </c>
-    </row>
-    <row r="511" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F510">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>6</v>
       </c>
@@ -52064,8 +52400,11 @@
       <c r="E511">
         <v>34</v>
       </c>
-    </row>
-    <row r="512" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F511">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>6</v>
       </c>
@@ -52081,8 +52420,11 @@
       <c r="E512">
         <v>66</v>
       </c>
-    </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F512">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>6</v>
       </c>
@@ -52098,8 +52440,11 @@
       <c r="E513">
         <v>85</v>
       </c>
-    </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F513">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>6</v>
       </c>
@@ -52115,8 +52460,11 @@
       <c r="E514">
         <v>28</v>
       </c>
-    </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F514">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>6</v>
       </c>
@@ -52132,8 +52480,11 @@
       <c r="E515">
         <v>88</v>
       </c>
-    </row>
-    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F515">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>6</v>
       </c>
@@ -52149,8 +52500,11 @@
       <c r="E516">
         <v>32</v>
       </c>
-    </row>
-    <row r="517" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F516">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
         <v>6</v>
       </c>
@@ -52166,8 +52520,11 @@
       <c r="E517">
         <v>61</v>
       </c>
-    </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F517">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
         <v>6</v>
       </c>
@@ -52183,8 +52540,11 @@
       <c r="E518">
         <v>87</v>
       </c>
-    </row>
-    <row r="519" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F518">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>6</v>
       </c>
@@ -52200,8 +52560,11 @@
       <c r="E519">
         <v>58</v>
       </c>
-    </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F519">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
         <v>6</v>
       </c>
@@ -52217,8 +52580,11 @@
       <c r="E520">
         <v>72</v>
       </c>
-    </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F520">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>6</v>
       </c>
@@ -52234,8 +52600,11 @@
       <c r="E521">
         <v>55</v>
       </c>
-    </row>
-    <row r="522" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F521">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
         <v>6</v>
       </c>
@@ -52251,8 +52620,11 @@
       <c r="E522">
         <v>68</v>
       </c>
-    </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F522">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
         <v>6</v>
       </c>
@@ -52268,8 +52640,11 @@
       <c r="E523">
         <v>3</v>
       </c>
-    </row>
-    <row r="524" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F523">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A524" t="s">
         <v>6</v>
       </c>
@@ -52285,8 +52660,11 @@
       <c r="E524">
         <v>70</v>
       </c>
-    </row>
-    <row r="525" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F524">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
         <v>6</v>
       </c>
@@ -52302,8 +52680,11 @@
       <c r="E525">
         <v>33</v>
       </c>
-    </row>
-    <row r="526" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F525">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A526" t="s">
         <v>6</v>
       </c>
@@ -52319,8 +52700,11 @@
       <c r="E526">
         <v>37</v>
       </c>
-    </row>
-    <row r="527" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F526">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
         <v>6</v>
       </c>
@@ -52336,8 +52720,11 @@
       <c r="E527">
         <v>93</v>
       </c>
-    </row>
-    <row r="528" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F527">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A528" t="s">
         <v>6</v>
       </c>
@@ -52353,8 +52740,11 @@
       <c r="E528">
         <v>21</v>
       </c>
-    </row>
-    <row r="529" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F528">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
         <v>6</v>
       </c>
@@ -52370,8 +52760,11 @@
       <c r="E529">
         <v>5</v>
       </c>
-    </row>
-    <row r="530" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F529">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
         <v>6</v>
       </c>
@@ -52387,8 +52780,11 @@
       <c r="E530">
         <v>69</v>
       </c>
-    </row>
-    <row r="531" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F530">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>6</v>
       </c>
@@ -52404,8 +52800,11 @@
       <c r="E531">
         <v>25</v>
       </c>
-    </row>
-    <row r="532" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F531">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>6</v>
       </c>
@@ -52421,8 +52820,11 @@
       <c r="E532">
         <v>41</v>
       </c>
-    </row>
-    <row r="533" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F532">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>6</v>
       </c>
@@ -52438,8 +52840,11 @@
       <c r="E533">
         <v>77</v>
       </c>
-    </row>
-    <row r="534" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F533">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
         <v>6</v>
       </c>
@@ -52455,8 +52860,11 @@
       <c r="E534">
         <v>80</v>
       </c>
-    </row>
-    <row r="535" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F534">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>6</v>
       </c>
@@ -52472,8 +52880,11 @@
       <c r="E535">
         <v>60</v>
       </c>
-    </row>
-    <row r="536" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F535">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
         <v>6</v>
       </c>
@@ -52489,8 +52900,11 @@
       <c r="E536">
         <v>67</v>
       </c>
-    </row>
-    <row r="537" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F536">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>6</v>
       </c>
@@ -52506,8 +52920,11 @@
       <c r="E537">
         <v>10</v>
       </c>
-    </row>
-    <row r="538" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F537">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
         <v>6</v>
       </c>
@@ -52523,8 +52940,11 @@
       <c r="E538">
         <v>57</v>
       </c>
-    </row>
-    <row r="539" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F538">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>6</v>
       </c>
@@ -52540,8 +52960,11 @@
       <c r="E539">
         <v>48</v>
       </c>
-    </row>
-    <row r="540" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F539">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>6</v>
       </c>
@@ -52557,8 +52980,11 @@
       <c r="E540">
         <v>5</v>
       </c>
-    </row>
-    <row r="541" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F540">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>6</v>
       </c>
@@ -52574,8 +53000,11 @@
       <c r="E541">
         <v>40</v>
       </c>
-    </row>
-    <row r="542" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F541">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
         <v>6</v>
       </c>
@@ -52591,8 +53020,11 @@
       <c r="E542">
         <v>43</v>
       </c>
-    </row>
-    <row r="543" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F542">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
         <v>6</v>
       </c>
@@ -52608,8 +53040,11 @@
       <c r="E543">
         <v>70</v>
       </c>
-    </row>
-    <row r="544" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F543">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
         <v>6</v>
       </c>
@@ -52625,8 +53060,11 @@
       <c r="E544">
         <v>8</v>
       </c>
-    </row>
-    <row r="545" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F544">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
         <v>6</v>
       </c>
@@ -52642,8 +53080,11 @@
       <c r="E545">
         <v>91</v>
       </c>
-    </row>
-    <row r="546" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F545">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
         <v>6</v>
       </c>
@@ -52659,8 +53100,11 @@
       <c r="E546">
         <v>73</v>
       </c>
-    </row>
-    <row r="547" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F546">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>6</v>
       </c>
@@ -52676,8 +53120,11 @@
       <c r="E547">
         <v>58</v>
       </c>
-    </row>
-    <row r="548" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F547">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A548" t="s">
         <v>6</v>
       </c>
@@ -52693,8 +53140,11 @@
       <c r="E548">
         <v>16</v>
       </c>
-    </row>
-    <row r="549" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F548">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A549" t="s">
         <v>6</v>
       </c>
@@ -52710,8 +53160,11 @@
       <c r="E549">
         <v>43</v>
       </c>
-    </row>
-    <row r="550" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F549">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A550" t="s">
         <v>6</v>
       </c>
@@ -52727,8 +53180,11 @@
       <c r="E550">
         <v>75</v>
       </c>
-    </row>
-    <row r="551" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F550">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A551" t="s">
         <v>6</v>
       </c>
@@ -52744,8 +53200,11 @@
       <c r="E551">
         <v>72</v>
       </c>
-    </row>
-    <row r="552" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F551">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A552" t="s">
         <v>6</v>
       </c>
@@ -52761,8 +53220,11 @@
       <c r="E552">
         <v>20</v>
       </c>
-    </row>
-    <row r="553" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F552">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
         <v>6</v>
       </c>
@@ -52778,8 +53240,11 @@
       <c r="E553">
         <v>21</v>
       </c>
-    </row>
-    <row r="554" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F553">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A554" t="s">
         <v>6</v>
       </c>
@@ -52795,8 +53260,11 @@
       <c r="E554">
         <v>19</v>
       </c>
-    </row>
-    <row r="555" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F554">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A555" t="s">
         <v>6</v>
       </c>
@@ -52812,8 +53280,11 @@
       <c r="E555">
         <v>83</v>
       </c>
-    </row>
-    <row r="556" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F555">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
         <v>6</v>
       </c>
@@ -52829,8 +53300,11 @@
       <c r="E556">
         <v>93</v>
       </c>
-    </row>
-    <row r="557" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F556">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
         <v>6</v>
       </c>
@@ -52846,8 +53320,11 @@
       <c r="E557">
         <v>35</v>
       </c>
-    </row>
-    <row r="558" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F557">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
         <v>6</v>
       </c>
@@ -52863,8 +53340,11 @@
       <c r="E558">
         <v>74</v>
       </c>
-    </row>
-    <row r="559" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F558">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
         <v>6</v>
       </c>
@@ -52880,8 +53360,11 @@
       <c r="E559">
         <v>43</v>
       </c>
-    </row>
-    <row r="560" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F559">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A560" t="s">
         <v>6</v>
       </c>
@@ -52897,8 +53380,11 @@
       <c r="E560">
         <v>55</v>
       </c>
-    </row>
-    <row r="561" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F560">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
         <v>6</v>
       </c>
@@ -52914,8 +53400,11 @@
       <c r="E561">
         <v>12</v>
       </c>
-    </row>
-    <row r="562" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F561">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A562" t="s">
         <v>6</v>
       </c>
@@ -52931,8 +53420,11 @@
       <c r="E562">
         <v>53</v>
       </c>
-    </row>
-    <row r="563" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F562">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A563" t="s">
         <v>6</v>
       </c>
@@ -52948,8 +53440,11 @@
       <c r="E563">
         <v>96</v>
       </c>
-    </row>
-    <row r="564" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F563">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A564" t="s">
         <v>6</v>
       </c>
@@ -52965,8 +53460,11 @@
       <c r="E564">
         <v>28</v>
       </c>
-    </row>
-    <row r="565" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F564">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A565" t="s">
         <v>6</v>
       </c>
@@ -52982,8 +53480,11 @@
       <c r="E565">
         <v>96</v>
       </c>
-    </row>
-    <row r="566" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F565">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A566" t="s">
         <v>6</v>
       </c>
@@ -52999,8 +53500,11 @@
       <c r="E566">
         <v>68</v>
       </c>
-    </row>
-    <row r="567" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F566">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A567" t="s">
         <v>6</v>
       </c>
@@ -53016,8 +53520,11 @@
       <c r="E567">
         <v>38</v>
       </c>
-    </row>
-    <row r="568" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F567">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A568" t="s">
         <v>6</v>
       </c>
@@ -53033,8 +53540,11 @@
       <c r="E568">
         <v>68</v>
       </c>
-    </row>
-    <row r="569" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F568">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A569" t="s">
         <v>6</v>
       </c>
@@ -53050,8 +53560,11 @@
       <c r="E569">
         <v>54</v>
       </c>
-    </row>
-    <row r="570" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F569">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="570" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
         <v>6</v>
       </c>
@@ -53067,8 +53580,11 @@
       <c r="E570">
         <v>26</v>
       </c>
-    </row>
-    <row r="571" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F570">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="571" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
         <v>6</v>
       </c>
@@ -53084,8 +53600,11 @@
       <c r="E571">
         <v>47</v>
       </c>
-    </row>
-    <row r="572" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F571">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="572" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
         <v>6</v>
       </c>
@@ -53101,8 +53620,11 @@
       <c r="E572">
         <v>14</v>
       </c>
-    </row>
-    <row r="573" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F572">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="573" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
         <v>6</v>
       </c>
@@ -53118,8 +53640,11 @@
       <c r="E573">
         <v>66</v>
       </c>
-    </row>
-    <row r="574" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F573">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="574" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
         <v>6</v>
       </c>
@@ -53135,8 +53660,11 @@
       <c r="E574">
         <v>47</v>
       </c>
-    </row>
-    <row r="575" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F574">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="575" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
         <v>6</v>
       </c>
@@ -53152,8 +53680,11 @@
       <c r="E575">
         <v>59</v>
       </c>
-    </row>
-    <row r="576" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F575">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="576" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A576" t="s">
         <v>6</v>
       </c>
@@ -53169,8 +53700,11 @@
       <c r="E576">
         <v>7</v>
       </c>
-    </row>
-    <row r="577" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F576">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="577" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>6</v>
       </c>
@@ -53186,8 +53720,11 @@
       <c r="E577">
         <v>45</v>
       </c>
-    </row>
-    <row r="578" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F577">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="578" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>6</v>
       </c>
@@ -53203,8 +53740,11 @@
       <c r="E578">
         <v>61</v>
       </c>
-    </row>
-    <row r="579" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F578">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="579" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
         <v>6</v>
       </c>
@@ -53220,8 +53760,11 @@
       <c r="E579">
         <v>54</v>
       </c>
-    </row>
-    <row r="580" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F579">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="580" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>6</v>
       </c>
@@ -53237,8 +53780,11 @@
       <c r="E580">
         <v>13</v>
       </c>
-    </row>
-    <row r="581" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F580">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="581" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>6</v>
       </c>
@@ -53254,8 +53800,11 @@
       <c r="E581">
         <v>89</v>
       </c>
-    </row>
-    <row r="582" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F581">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="582" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>6</v>
       </c>
@@ -53271,8 +53820,11 @@
       <c r="E582">
         <v>77</v>
       </c>
-    </row>
-    <row r="583" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F582">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>6</v>
       </c>
@@ -53289,7 +53841,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="584" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>6</v>
       </c>
@@ -53306,7 +53858,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="585" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>6</v>
       </c>
@@ -53323,7 +53875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="586" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
         <v>6</v>
       </c>
@@ -53340,7 +53892,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="587" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>6</v>
       </c>
@@ -53357,7 +53909,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="588" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
         <v>6</v>
       </c>
@@ -53374,7 +53926,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="589" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>6</v>
       </c>
@@ -53391,7 +53943,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="590" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
         <v>6</v>
       </c>
@@ -53408,7 +53960,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="591" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
         <v>6</v>
       </c>
@@ -53425,7 +53977,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="592" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
update da target nos testes
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Documents\GitHub\22-2b-cd-p1-grupo_joaoogp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72378759-B21A-47BB-A5C8-3482E4BBCCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87529DFC-5143-4237-AA8A-2C467DA4052C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
     <sheet name="Teste" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8016" uniqueCount="5894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8015" uniqueCount="5893">
   <si>
     <t>Categoria</t>
   </si>
@@ -17700,9 +17713,6 @@
   </si>
   <si>
     <t>neutra</t>
-  </si>
-  <si>
-    <t>[]</t>
   </si>
 </sst>
 </file>
@@ -17769,15 +17779,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18118,8 +18127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1201"/>
   <sheetViews>
-    <sheetView topLeftCell="A792" workbookViewId="0">
-      <selection activeCell="I806" sqref="I806"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18143,13 +18152,13 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>5890</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>5892</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>5891</v>
       </c>
     </row>
@@ -18172,13 +18181,13 @@
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
         <v>2</v>
       </c>
     </row>
@@ -34201,7 +34210,7 @@
       <c r="F803">
         <v>1</v>
       </c>
-      <c r="K803" s="3"/>
+      <c r="K803" s="2"/>
     </row>
     <row r="804" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A804" t="s">
@@ -42174,8 +42183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H801"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A572" workbookViewId="0">
-      <selection activeCell="F582" sqref="F582"/>
+    <sheetView topLeftCell="A574" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G583" sqref="G583"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42279,7 +42288,7 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -50181,7 +50190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="401" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>6</v>
       </c>
@@ -50201,7 +50210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="402" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>6</v>
       </c>
@@ -50220,11 +50229,8 @@
       <c r="F402">
         <v>1</v>
       </c>
-      <c r="G402" t="s">
-        <v>5893</v>
-      </c>
-    </row>
-    <row r="403" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>6</v>
       </c>
@@ -50244,7 +50250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="404" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>6</v>
       </c>
@@ -50264,7 +50270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="405" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>6</v>
       </c>
@@ -50284,7 +50290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="406" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>6</v>
       </c>
@@ -50304,7 +50310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="407" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>6</v>
       </c>
@@ -50324,7 +50330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>6</v>
       </c>
@@ -50344,7 +50350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>6</v>
       </c>
@@ -50364,7 +50370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>6</v>
       </c>
@@ -50384,7 +50390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="411" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>6</v>
       </c>
@@ -50404,7 +50410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="412" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>6</v>
       </c>
@@ -50424,7 +50430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>6</v>
       </c>
@@ -50444,7 +50450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>6</v>
       </c>
@@ -50464,7 +50470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>6</v>
       </c>
@@ -50484,7 +50490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>6</v>
       </c>
@@ -53840,6 +53846,9 @@
       <c r="E583">
         <v>53</v>
       </c>
+      <c r="F583">
+        <v>2</v>
+      </c>
     </row>
     <row r="584" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
@@ -53857,6 +53866,9 @@
       <c r="E584">
         <v>43</v>
       </c>
+      <c r="F584">
+        <v>1</v>
+      </c>
     </row>
     <row r="585" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
@@ -53874,6 +53886,9 @@
       <c r="E585">
         <v>13</v>
       </c>
+      <c r="F585">
+        <v>1</v>
+      </c>
     </row>
     <row r="586" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
@@ -53891,6 +53906,9 @@
       <c r="E586">
         <v>43</v>
       </c>
+      <c r="F586">
+        <v>1</v>
+      </c>
     </row>
     <row r="587" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
@@ -53908,6 +53926,9 @@
       <c r="E587">
         <v>75</v>
       </c>
+      <c r="F587">
+        <v>0</v>
+      </c>
     </row>
     <row r="588" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
@@ -53925,6 +53946,9 @@
       <c r="E588">
         <v>44</v>
       </c>
+      <c r="F588">
+        <v>1</v>
+      </c>
     </row>
     <row r="589" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
@@ -53942,6 +53966,9 @@
       <c r="E589">
         <v>53</v>
       </c>
+      <c r="F589">
+        <v>1</v>
+      </c>
     </row>
     <row r="590" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
@@ -53959,6 +53986,9 @@
       <c r="E590">
         <v>21</v>
       </c>
+      <c r="F590">
+        <v>1</v>
+      </c>
     </row>
     <row r="591" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
@@ -53976,6 +54006,9 @@
       <c r="E591">
         <v>26</v>
       </c>
+      <c r="F591">
+        <v>1</v>
+      </c>
     </row>
     <row r="592" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
@@ -53993,8 +54026,11 @@
       <c r="E592">
         <v>27</v>
       </c>
-    </row>
-    <row r="593" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F592">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="593" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
         <v>6</v>
       </c>
@@ -54010,8 +54046,11 @@
       <c r="E593">
         <v>14</v>
       </c>
-    </row>
-    <row r="594" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F593">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="594" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A594" t="s">
         <v>6</v>
       </c>
@@ -54027,8 +54066,11 @@
       <c r="E594">
         <v>65</v>
       </c>
-    </row>
-    <row r="595" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F594">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="595" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
         <v>6</v>
       </c>
@@ -54044,8 +54086,11 @@
       <c r="E595">
         <v>54</v>
       </c>
-    </row>
-    <row r="596" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F595">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="596" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
         <v>6</v>
       </c>
@@ -54061,8 +54106,11 @@
       <c r="E596">
         <v>15</v>
       </c>
-    </row>
-    <row r="597" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F596">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="597" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
         <v>6</v>
       </c>
@@ -54078,8 +54126,11 @@
       <c r="E597">
         <v>59</v>
       </c>
-    </row>
-    <row r="598" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F597">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="598" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
         <v>6</v>
       </c>
@@ -54095,8 +54146,11 @@
       <c r="E598">
         <v>29</v>
       </c>
-    </row>
-    <row r="599" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F598">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="599" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
         <v>6</v>
       </c>
@@ -54112,8 +54166,11 @@
       <c r="E599">
         <v>38</v>
       </c>
-    </row>
-    <row r="600" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F599">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="600" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
         <v>6</v>
       </c>
@@ -54129,8 +54186,11 @@
       <c r="E600">
         <v>91</v>
       </c>
-    </row>
-    <row r="601" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F600">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="601" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
         <v>6</v>
       </c>
@@ -54146,8 +54206,11 @@
       <c r="E601">
         <v>99</v>
       </c>
-    </row>
-    <row r="602" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F601">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="602" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
         <v>6</v>
       </c>
@@ -54163,8 +54226,11 @@
       <c r="E602">
         <v>49</v>
       </c>
-    </row>
-    <row r="603" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F602">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="603" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
         <v>6</v>
       </c>
@@ -54180,8 +54246,11 @@
       <c r="E603">
         <v>74</v>
       </c>
-    </row>
-    <row r="604" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F603">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="604" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
         <v>6</v>
       </c>
@@ -54197,8 +54266,11 @@
       <c r="E604">
         <v>30</v>
       </c>
-    </row>
-    <row r="605" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F604">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
         <v>6</v>
       </c>
@@ -54214,8 +54286,11 @@
       <c r="E605">
         <v>62</v>
       </c>
-    </row>
-    <row r="606" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F605">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="606" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A606" t="s">
         <v>6</v>
       </c>
@@ -54231,8 +54306,11 @@
       <c r="E606">
         <v>47</v>
       </c>
-    </row>
-    <row r="607" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F606">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="607" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
         <v>6</v>
       </c>
@@ -54248,8 +54326,11 @@
       <c r="E607">
         <v>28</v>
       </c>
-    </row>
-    <row r="608" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F607">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="608" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
         <v>6</v>
       </c>
@@ -54265,8 +54346,11 @@
       <c r="E608">
         <v>93</v>
       </c>
-    </row>
-    <row r="609" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F608">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="609" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A609" t="s">
         <v>6</v>
       </c>
@@ -54282,8 +54366,11 @@
       <c r="E609">
         <v>73</v>
       </c>
-    </row>
-    <row r="610" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F609">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="610" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A610" t="s">
         <v>6</v>
       </c>
@@ -54299,8 +54386,11 @@
       <c r="E610">
         <v>74</v>
       </c>
-    </row>
-    <row r="611" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F610">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="611" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A611" t="s">
         <v>6</v>
       </c>
@@ -54316,8 +54406,11 @@
       <c r="E611">
         <v>59</v>
       </c>
-    </row>
-    <row r="612" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F611">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="612" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A612" t="s">
         <v>6</v>
       </c>
@@ -54333,8 +54426,11 @@
       <c r="E612">
         <v>92</v>
       </c>
-    </row>
-    <row r="613" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F612">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="613" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A613" t="s">
         <v>6</v>
       </c>
@@ -54350,8 +54446,11 @@
       <c r="E613">
         <v>20</v>
       </c>
-    </row>
-    <row r="614" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F613">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="614" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A614" t="s">
         <v>6</v>
       </c>
@@ -54367,8 +54466,11 @@
       <c r="E614">
         <v>97</v>
       </c>
-    </row>
-    <row r="615" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F614">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="615" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A615" t="s">
         <v>6</v>
       </c>
@@ -54384,8 +54486,11 @@
       <c r="E615">
         <v>42</v>
       </c>
-    </row>
-    <row r="616" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F615">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="616" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A616" t="s">
         <v>6</v>
       </c>
@@ -54401,8 +54506,11 @@
       <c r="E616">
         <v>79</v>
       </c>
-    </row>
-    <row r="617" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F616">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="617" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A617" t="s">
         <v>6</v>
       </c>
@@ -54418,8 +54526,11 @@
       <c r="E617">
         <v>12</v>
       </c>
-    </row>
-    <row r="618" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F617">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="618" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A618" t="s">
         <v>6</v>
       </c>
@@ -54435,8 +54546,11 @@
       <c r="E618">
         <v>50</v>
       </c>
-    </row>
-    <row r="619" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F618">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
         <v>6</v>
       </c>
@@ -54452,8 +54566,11 @@
       <c r="E619">
         <v>99</v>
       </c>
-    </row>
-    <row r="620" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F619">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A620" t="s">
         <v>6</v>
       </c>
@@ -54469,8 +54586,11 @@
       <c r="E620">
         <v>99</v>
       </c>
-    </row>
-    <row r="621" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F620">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="621" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A621" t="s">
         <v>6</v>
       </c>
@@ -54486,8 +54606,11 @@
       <c r="E621">
         <v>86</v>
       </c>
-    </row>
-    <row r="622" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F621">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="622" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A622" t="s">
         <v>6</v>
       </c>
@@ -54503,8 +54626,11 @@
       <c r="E622">
         <v>53</v>
       </c>
-    </row>
-    <row r="623" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F622">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="623" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A623" t="s">
         <v>6</v>
       </c>
@@ -54520,8 +54646,11 @@
       <c r="E623">
         <v>90</v>
       </c>
-    </row>
-    <row r="624" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F623">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="624" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A624" t="s">
         <v>6</v>
       </c>
@@ -54536,6 +54665,9 @@
       </c>
       <c r="E624">
         <v>58</v>
+      </c>
+      <c r="F624">
+        <v>0</v>
       </c>
     </row>
     <row r="625" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Correção da planilha de dados
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Documents\GitHub\22-2b-cd-p1-grupo_joaoogp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87529DFC-5143-4237-AA8A-2C467DA4052C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F51F05-A453-4CB1-883F-F034C5C47115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="10524" windowHeight="7860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8015" uniqueCount="5893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8012" uniqueCount="5890">
   <si>
     <t>Categoria</t>
   </si>
@@ -17704,15 +17704,6 @@
   </si>
   <si>
     <t>18/08/2022 15:51</t>
-  </si>
-  <si>
-    <t>negativa</t>
-  </si>
-  <si>
-    <t>positiva</t>
-  </si>
-  <si>
-    <t>neutra</t>
   </si>
 </sst>
 </file>
@@ -17779,14 +17770,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18127,13 +18116,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18152,17 +18141,8 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>5890</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5892</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5891</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -18181,17 +18161,8 @@
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="I2" s="4">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -18211,7 +18182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -18231,7 +18202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -18251,7 +18222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -18271,7 +18242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -18291,7 +18262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -18311,7 +18282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -18331,7 +18302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -18351,7 +18322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -18371,7 +18342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -18391,7 +18362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -18411,7 +18382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -18431,7 +18402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -18451,7 +18422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -34271,7 +34242,6 @@
       <c r="F806">
         <v>1</v>
       </c>
-      <c r="I806" s="3"/>
     </row>
     <row r="807" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A807" t="s">
@@ -42183,7 +42153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H801"/>
   <sheetViews>
-    <sheetView topLeftCell="A574" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A578" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G583" sqref="G583"/>
     </sheetView>
   </sheetViews>
@@ -53710,7 +53680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="577" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>6</v>
       </c>
@@ -53730,7 +53700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="578" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>6</v>
       </c>
@@ -53750,7 +53720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="579" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
         <v>6</v>
       </c>
@@ -53770,7 +53740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="580" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>6</v>
       </c>
@@ -53790,7 +53760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="581" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>6</v>
       </c>
@@ -53810,7 +53780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="582" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>6</v>
       </c>
@@ -53830,7 +53800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="583" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>6</v>
       </c>
@@ -53849,8 +53819,9 @@
       <c r="F583">
         <v>2</v>
       </c>
-    </row>
-    <row r="584" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G583" s="2"/>
+    </row>
+    <row r="584" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>6</v>
       </c>
@@ -53870,7 +53841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="585" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>6</v>
       </c>
@@ -53890,7 +53861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="586" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
         <v>6</v>
       </c>
@@ -53910,7 +53881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="587" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>6</v>
       </c>
@@ -53930,7 +53901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="588" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
         <v>6</v>
       </c>
@@ -53950,7 +53921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="589" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>6</v>
       </c>
@@ -53970,7 +53941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="590" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
         <v>6</v>
       </c>
@@ -53990,7 +53961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="591" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
         <v>6</v>
       </c>
@@ -54010,7 +53981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="592" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
         <v>6</v>
       </c>

</xml_diff>